<commit_message>
Including the initial beats
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/attempt1.xlsx
+++ b/R peak detection/beatdetection/attempt1.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -445,31 +445,31 @@
         <v>100</v>
       </c>
       <c r="B1" t="n">
-        <v>2269</v>
+        <v>2272</v>
       </c>
       <c r="C1" t="n">
         <v>2272</v>
       </c>
       <c r="D1" t="n">
-        <v>2268</v>
+        <v>2271</v>
       </c>
       <c r="E1" t="n">
         <v>0</v>
       </c>
       <c r="F1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G1" t="n">
-        <v>99.86789960369882</v>
+        <v>100</v>
       </c>
       <c r="H1" t="n">
         <v>100</v>
       </c>
       <c r="I1" t="n">
-        <v>0.001320422535211268</v>
+        <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>37.84133243560791</v>
+        <v>37.63093018531799</v>
       </c>
     </row>
     <row r="2">
@@ -477,31 +477,31 @@
         <v>101</v>
       </c>
       <c r="B2" t="n">
-        <v>1863</v>
+        <v>1865</v>
       </c>
       <c r="C2" t="n">
         <v>1864</v>
       </c>
       <c r="D2" t="n">
-        <v>1860</v>
+        <v>1863</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>99.8389694041868</v>
+        <v>100</v>
       </c>
       <c r="H2" t="n">
-        <v>99.89258861439312</v>
+        <v>99.94635193133047</v>
       </c>
       <c r="I2" t="n">
-        <v>0.002682403433476395</v>
+        <v>0.000536480686695279</v>
       </c>
       <c r="J2" t="n">
-        <v>38.70834493637085</v>
+        <v>38.19485068321228</v>
       </c>
     </row>
     <row r="3">
@@ -509,31 +509,31 @@
         <v>102</v>
       </c>
       <c r="B3" t="n">
-        <v>2183</v>
+        <v>2186</v>
       </c>
       <c r="C3" t="n">
         <v>2186</v>
       </c>
       <c r="D3" t="n">
-        <v>2182</v>
+        <v>2185</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>99.86270022883295</v>
+        <v>100</v>
       </c>
       <c r="H3" t="n">
         <v>100</v>
       </c>
       <c r="I3" t="n">
-        <v>0.001372369624885636</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>38.40542101860046</v>
+        <v>38.67928028106689</v>
       </c>
     </row>
     <row r="4">
@@ -541,31 +541,31 @@
         <v>103</v>
       </c>
       <c r="B4" t="n">
-        <v>2080</v>
+        <v>2083</v>
       </c>
       <c r="C4" t="n">
         <v>2084</v>
       </c>
       <c r="D4" t="n">
-        <v>2079</v>
+        <v>2082</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>99.80796927508402</v>
+        <v>99.951992318771</v>
       </c>
       <c r="H4" t="n">
         <v>100</v>
       </c>
       <c r="I4" t="n">
-        <v>0.001919385796545105</v>
+        <v>0.0004798464491362764</v>
       </c>
       <c r="J4" t="n">
-        <v>39.13652944564819</v>
+        <v>39.04195380210876</v>
       </c>
     </row>
     <row r="5">
@@ -573,31 +573,31 @@
         <v>104</v>
       </c>
       <c r="B5" t="n">
-        <v>2242</v>
+        <v>2245</v>
       </c>
       <c r="C5" t="n">
         <v>2228</v>
       </c>
       <c r="D5" t="n">
-        <v>2223</v>
+        <v>2226</v>
       </c>
       <c r="E5" t="n">
         <v>18</v>
       </c>
       <c r="F5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>99.82038616973507</v>
+        <v>99.95509654243376</v>
       </c>
       <c r="H5" t="n">
-        <v>99.19678714859438</v>
+        <v>99.19786096256685</v>
       </c>
       <c r="I5" t="n">
-        <v>0.009874326750448833</v>
+        <v>0.008527827648114902</v>
       </c>
       <c r="J5" t="n">
-        <v>38.94820618629456</v>
+        <v>39.25133323669434</v>
       </c>
     </row>
     <row r="6">
@@ -605,31 +605,31 @@
         <v>105</v>
       </c>
       <c r="B6" t="n">
-        <v>2576</v>
+        <v>2580</v>
       </c>
       <c r="C6" t="n">
         <v>2571</v>
       </c>
       <c r="D6" t="n">
-        <v>2557</v>
+        <v>2561</v>
       </c>
       <c r="E6" t="n">
         <v>18</v>
       </c>
       <c r="F6" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G6" t="n">
-        <v>99.49416342412451</v>
+        <v>99.64980544747081</v>
       </c>
       <c r="H6" t="n">
-        <v>99.30097087378641</v>
+        <v>99.30205506010081</v>
       </c>
       <c r="I6" t="n">
-        <v>0.01205756514974718</v>
+        <v>0.01050175029171529</v>
       </c>
       <c r="J6" t="n">
-        <v>39.84603476524353</v>
+        <v>39.79677248001099</v>
       </c>
     </row>
     <row r="7">
@@ -637,31 +637,31 @@
         <v>106</v>
       </c>
       <c r="B7" t="n">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C7" t="n">
         <v>2027</v>
       </c>
       <c r="D7" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G7" t="n">
-        <v>99.75320829220138</v>
+        <v>99.85192497532083</v>
       </c>
       <c r="H7" t="n">
         <v>100</v>
       </c>
       <c r="I7" t="n">
-        <v>0.00246669955599408</v>
+        <v>0.001480019733596448</v>
       </c>
       <c r="J7" t="n">
-        <v>39.62533712387085</v>
+        <v>39.46328949928284</v>
       </c>
     </row>
     <row r="8">
@@ -669,31 +669,31 @@
         <v>107</v>
       </c>
       <c r="B8" t="n">
-        <v>2159</v>
+        <v>2162</v>
       </c>
       <c r="C8" t="n">
         <v>2135</v>
       </c>
       <c r="D8" t="n">
-        <v>2131</v>
+        <v>2133</v>
       </c>
       <c r="E8" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>99.85941893158387</v>
+        <v>99.95313964386129</v>
       </c>
       <c r="H8" t="n">
-        <v>98.74884151992586</v>
+        <v>98.7043035631652</v>
       </c>
       <c r="I8" t="n">
-        <v>0.01405152224824356</v>
+        <v>0.01358313817330211</v>
       </c>
       <c r="J8" t="n">
-        <v>40.28927421569824</v>
+        <v>40.28286266326904</v>
       </c>
     </row>
     <row r="9">
@@ -701,31 +701,31 @@
         <v>108</v>
       </c>
       <c r="B9" t="n">
-        <v>1801</v>
+        <v>1804</v>
       </c>
       <c r="C9" t="n">
         <v>1762</v>
       </c>
       <c r="D9" t="n">
-        <v>1751</v>
+        <v>1754</v>
       </c>
       <c r="E9" t="n">
         <v>49</v>
       </c>
       <c r="F9" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G9" t="n">
-        <v>99.43214082907438</v>
+        <v>99.60249858035208</v>
       </c>
       <c r="H9" t="n">
-        <v>97.27777777777777</v>
+        <v>97.28230726566834</v>
       </c>
       <c r="I9" t="n">
-        <v>0.03348467650397276</v>
+        <v>0.03178206583427923</v>
       </c>
       <c r="J9" t="n">
-        <v>39.21606922149658</v>
+        <v>39.54617071151733</v>
       </c>
     </row>
     <row r="10">
@@ -733,31 +733,31 @@
         <v>109</v>
       </c>
       <c r="B10" t="n">
-        <v>2521</v>
+        <v>2525</v>
       </c>
       <c r="C10" t="n">
         <v>2530</v>
       </c>
       <c r="D10" t="n">
-        <v>2520</v>
+        <v>2523</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G10" t="n">
-        <v>99.64412811387901</v>
+        <v>99.76275207591934</v>
       </c>
       <c r="H10" t="n">
-        <v>100</v>
+        <v>99.96038034865293</v>
       </c>
       <c r="I10" t="n">
-        <v>0.003557312252964427</v>
+        <v>0.002766798418972332</v>
       </c>
       <c r="J10" t="n">
-        <v>40.08057069778442</v>
+        <v>39.61692547798157</v>
       </c>
     </row>
     <row r="11">
@@ -765,31 +765,31 @@
         <v>111</v>
       </c>
       <c r="B11" t="n">
-        <v>2122</v>
+        <v>2125</v>
       </c>
       <c r="C11" t="n">
         <v>2124</v>
       </c>
       <c r="D11" t="n">
-        <v>2118</v>
+        <v>2121</v>
       </c>
       <c r="E11" t="n">
         <v>3</v>
       </c>
       <c r="F11" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
-        <v>99.76448422044277</v>
+        <v>99.90579368817711</v>
       </c>
       <c r="H11" t="n">
-        <v>99.85855728429986</v>
+        <v>99.85875706214689</v>
       </c>
       <c r="I11" t="n">
-        <v>0.003766478342749529</v>
+        <v>0.002354048964218456</v>
       </c>
       <c r="J11" t="n">
-        <v>39.33779859542847</v>
+        <v>39.57951736450195</v>
       </c>
     </row>
     <row r="12">
@@ -797,31 +797,31 @@
         <v>112</v>
       </c>
       <c r="B12" t="n">
-        <v>2542</v>
+        <v>2546</v>
       </c>
       <c r="C12" t="n">
         <v>2538</v>
       </c>
       <c r="D12" t="n">
-        <v>2533</v>
+        <v>2537</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
       </c>
       <c r="F12" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>99.84233346472212</v>
+        <v>100</v>
       </c>
       <c r="H12" t="n">
-        <v>99.68516332152696</v>
+        <v>99.68565815324165</v>
       </c>
       <c r="I12" t="n">
-        <v>0.004728132387706856</v>
+        <v>0.003152088258471237</v>
       </c>
       <c r="J12" t="n">
-        <v>39.44948768615723</v>
+        <v>39.15743851661682</v>
       </c>
     </row>
     <row r="13">
@@ -829,31 +829,31 @@
         <v>113</v>
       </c>
       <c r="B13" t="n">
-        <v>1795</v>
+        <v>1796</v>
       </c>
       <c r="C13" t="n">
         <v>1794</v>
       </c>
       <c r="D13" t="n">
-        <v>1791</v>
+        <v>1793</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>99.88845510317903</v>
+        <v>100</v>
       </c>
       <c r="H13" t="n">
-        <v>99.83277591973244</v>
+        <v>99.88857938718662</v>
       </c>
       <c r="I13" t="n">
-        <v>0.002787068004459309</v>
+        <v>0.001114827201783724</v>
       </c>
       <c r="J13" t="n">
-        <v>39.29853391647339</v>
+        <v>39.72747802734375</v>
       </c>
     </row>
     <row r="14">
@@ -861,31 +861,31 @@
         <v>114</v>
       </c>
       <c r="B14" t="n">
-        <v>1886</v>
+        <v>1887</v>
       </c>
       <c r="C14" t="n">
         <v>1879</v>
       </c>
       <c r="D14" t="n">
-        <v>1874</v>
+        <v>1876</v>
       </c>
       <c r="E14" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G14" t="n">
-        <v>99.78700745473908</v>
+        <v>99.89350372736955</v>
       </c>
       <c r="H14" t="n">
-        <v>99.41644562334217</v>
+        <v>99.46977730646871</v>
       </c>
       <c r="I14" t="n">
-        <v>0.007982969664715274</v>
+        <v>0.006386375731772219</v>
       </c>
       <c r="J14" t="n">
-        <v>38.74590587615967</v>
+        <v>38.87654781341553</v>
       </c>
     </row>
     <row r="15">
@@ -893,31 +893,31 @@
         <v>115</v>
       </c>
       <c r="B15" t="n">
-        <v>1950</v>
+        <v>1952</v>
       </c>
       <c r="C15" t="n">
         <v>1953</v>
       </c>
       <c r="D15" t="n">
-        <v>1949</v>
+        <v>1951</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>99.84631147540983</v>
+        <v>99.94877049180327</v>
       </c>
       <c r="H15" t="n">
         <v>100</v>
       </c>
       <c r="I15" t="n">
-        <v>0.001536098310291859</v>
+        <v>0.0005120327700972862</v>
       </c>
       <c r="J15" t="n">
-        <v>38.80195379257202</v>
+        <v>38.48779344558716</v>
       </c>
     </row>
     <row r="16">
@@ -925,31 +925,31 @@
         <v>116</v>
       </c>
       <c r="B16" t="n">
-        <v>2385</v>
+        <v>2389</v>
       </c>
       <c r="C16" t="n">
         <v>2411</v>
       </c>
       <c r="D16" t="n">
-        <v>2384</v>
+        <v>2387</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G16" t="n">
-        <v>98.92116182572614</v>
+        <v>99.04564315352697</v>
       </c>
       <c r="H16" t="n">
-        <v>100</v>
+        <v>99.95812395309883</v>
       </c>
       <c r="I16" t="n">
-        <v>0.01078390709249274</v>
+        <v>0.009954375777685608</v>
       </c>
       <c r="J16" t="n">
-        <v>40.05220150947571</v>
+        <v>40.73249101638794</v>
       </c>
     </row>
     <row r="17">
@@ -957,31 +957,31 @@
         <v>117</v>
       </c>
       <c r="B17" t="n">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="C17" t="n">
         <v>1534</v>
       </c>
       <c r="D17" t="n">
-        <v>1531</v>
+        <v>1533</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>99.86953685583822</v>
+        <v>100</v>
       </c>
       <c r="H17" t="n">
-        <v>99.86953685583822</v>
+        <v>99.9348109517601</v>
       </c>
       <c r="I17" t="n">
-        <v>0.002607561929595828</v>
+        <v>0.000651890482398957</v>
       </c>
       <c r="J17" t="n">
-        <v>39.25186538696289</v>
+        <v>39.60176634788513</v>
       </c>
     </row>
     <row r="18">
@@ -989,31 +989,31 @@
         <v>118</v>
       </c>
       <c r="B18" t="n">
-        <v>2276</v>
+        <v>2281</v>
       </c>
       <c r="C18" t="n">
         <v>2276</v>
       </c>
       <c r="D18" t="n">
-        <v>2272</v>
+        <v>2275</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>99.86813186813187</v>
+        <v>100</v>
       </c>
       <c r="H18" t="n">
-        <v>99.86813186813187</v>
+        <v>99.78070175438596</v>
       </c>
       <c r="I18" t="n">
-        <v>0.002636203866432337</v>
+        <v>0.002196836555360281</v>
       </c>
       <c r="J18" t="n">
-        <v>40.57055997848511</v>
+        <v>41.20593619346619</v>
       </c>
     </row>
     <row r="19">
@@ -1021,31 +1021,31 @@
         <v>119</v>
       </c>
       <c r="B19" t="n">
-        <v>1988</v>
+        <v>1990</v>
       </c>
       <c r="C19" t="n">
         <v>1987</v>
       </c>
       <c r="D19" t="n">
-        <v>1983</v>
+        <v>1986</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>99.84894259818731</v>
+        <v>100</v>
       </c>
       <c r="H19" t="n">
-        <v>99.79869149471565</v>
+        <v>99.84917043740573</v>
       </c>
       <c r="I19" t="n">
-        <v>0.003522898842476095</v>
+        <v>0.001509813789632612</v>
       </c>
       <c r="J19" t="n">
-        <v>39.53732848167419</v>
+        <v>42.99114060401917</v>
       </c>
     </row>
     <row r="20">
@@ -1053,31 +1053,31 @@
         <v>121</v>
       </c>
       <c r="B20" t="n">
-        <v>1859</v>
+        <v>1861</v>
       </c>
       <c r="C20" t="n">
         <v>1863</v>
       </c>
       <c r="D20" t="n">
-        <v>1858</v>
+        <v>1860</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G20" t="n">
-        <v>99.78517722878625</v>
+        <v>99.89258861439312</v>
       </c>
       <c r="H20" t="n">
         <v>100</v>
       </c>
       <c r="I20" t="n">
-        <v>0.002147074610842727</v>
+        <v>0.001073537305421363</v>
       </c>
       <c r="J20" t="n">
-        <v>38.76749730110168</v>
+        <v>38.84943127632141</v>
       </c>
     </row>
     <row r="21">
@@ -1085,31 +1085,31 @@
         <v>122</v>
       </c>
       <c r="B21" t="n">
-        <v>2470</v>
+        <v>2475</v>
       </c>
       <c r="C21" t="n">
         <v>2474</v>
       </c>
       <c r="D21" t="n">
-        <v>2469</v>
+        <v>2473</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>99.83825313384553</v>
+        <v>100</v>
       </c>
       <c r="H21" t="n">
-        <v>100</v>
+        <v>99.95957962813257</v>
       </c>
       <c r="I21" t="n">
-        <v>0.001616814874696847</v>
+        <v>0.0004042037186742118</v>
       </c>
       <c r="J21" t="n">
-        <v>39.33477187156677</v>
+        <v>39.91568899154663</v>
       </c>
     </row>
     <row r="22">
@@ -1117,31 +1117,31 @@
         <v>123</v>
       </c>
       <c r="B22" t="n">
-        <v>1516</v>
+        <v>1519</v>
       </c>
       <c r="C22" t="n">
         <v>1517</v>
       </c>
       <c r="D22" t="n">
-        <v>1514</v>
+        <v>1516</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>99.86807387862797</v>
+        <v>100</v>
       </c>
       <c r="H22" t="n">
-        <v>99.93399339933994</v>
+        <v>99.86824769433466</v>
       </c>
       <c r="I22" t="n">
-        <v>0.001977587343441002</v>
+        <v>0.001318391562294001</v>
       </c>
       <c r="J22" t="n">
-        <v>38.93475031852722</v>
+        <v>39.1142258644104</v>
       </c>
     </row>
     <row r="23">
@@ -1149,31 +1149,31 @@
         <v>124</v>
       </c>
       <c r="B23" t="n">
-        <v>1617</v>
+        <v>1619</v>
       </c>
       <c r="C23" t="n">
         <v>1619</v>
       </c>
       <c r="D23" t="n">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G23" t="n">
-        <v>99.87639060568603</v>
+        <v>99.93819530284301</v>
       </c>
       <c r="H23" t="n">
-        <v>100</v>
+        <v>99.93819530284301</v>
       </c>
       <c r="I23" t="n">
         <v>0.001235330450895615</v>
       </c>
       <c r="J23" t="n">
-        <v>39.12248873710632</v>
+        <v>39.34931707382202</v>
       </c>
     </row>
     <row r="24">
@@ -1181,31 +1181,31 @@
         <v>200</v>
       </c>
       <c r="B24" t="n">
-        <v>2603</v>
+        <v>2608</v>
       </c>
       <c r="C24" t="n">
         <v>2600</v>
       </c>
       <c r="D24" t="n">
-        <v>2594</v>
+        <v>2598</v>
       </c>
       <c r="E24" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F24" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>99.80761831473643</v>
+        <v>99.96152366294729</v>
       </c>
       <c r="H24" t="n">
-        <v>99.69254419677172</v>
+        <v>99.6547756041427</v>
       </c>
       <c r="I24" t="n">
-        <v>0.005</v>
+        <v>0.003846153846153846</v>
       </c>
       <c r="J24" t="n">
-        <v>39.67539715766907</v>
+        <v>40.02467513084412</v>
       </c>
     </row>
     <row r="25">
@@ -1213,31 +1213,31 @@
         <v>201</v>
       </c>
       <c r="B25" t="n">
-        <v>1949</v>
+        <v>1954</v>
       </c>
       <c r="C25" t="n">
         <v>1963</v>
       </c>
       <c r="D25" t="n">
-        <v>1946</v>
+        <v>1951</v>
       </c>
       <c r="E25" t="n">
         <v>2</v>
       </c>
       <c r="F25" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G25" t="n">
-        <v>99.18450560652396</v>
+        <v>99.43934760448522</v>
       </c>
       <c r="H25" t="n">
-        <v>99.89733059548254</v>
+        <v>99.89759344598055</v>
       </c>
       <c r="I25" t="n">
-        <v>0.009169638308711156</v>
+        <v>0.006622516556291391</v>
       </c>
       <c r="J25" t="n">
-        <v>38.40084624290466</v>
+        <v>38.52096438407898</v>
       </c>
     </row>
     <row r="26">
@@ -1245,31 +1245,31 @@
         <v>202</v>
       </c>
       <c r="B26" t="n">
-        <v>2125</v>
+        <v>2127</v>
       </c>
       <c r="C26" t="n">
         <v>2136</v>
       </c>
       <c r="D26" t="n">
-        <v>2123</v>
+        <v>2125</v>
       </c>
       <c r="E26" t="n">
         <v>1</v>
       </c>
       <c r="F26" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G26" t="n">
-        <v>99.43793911007026</v>
+        <v>99.53161592505855</v>
       </c>
       <c r="H26" t="n">
-        <v>99.95291902071563</v>
+        <v>99.95296331138287</v>
       </c>
       <c r="I26" t="n">
-        <v>0.006086142322097378</v>
+        <v>0.005149812734082397</v>
       </c>
       <c r="J26" t="n">
-        <v>38.82582139968872</v>
+        <v>38.76453590393066</v>
       </c>
     </row>
     <row r="27">
@@ -1277,31 +1277,31 @@
         <v>203</v>
       </c>
       <c r="B27" t="n">
-        <v>2920</v>
+        <v>2926</v>
       </c>
       <c r="C27" t="n">
         <v>2977</v>
       </c>
       <c r="D27" t="n">
-        <v>2899</v>
+        <v>2902</v>
       </c>
       <c r="E27" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F27" t="n">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G27" t="n">
-        <v>97.41263440860214</v>
+        <v>97.51344086021506</v>
       </c>
       <c r="H27" t="n">
-        <v>99.31483384720795</v>
+        <v>99.21367521367522</v>
       </c>
       <c r="I27" t="n">
         <v>0.03258313738663084</v>
       </c>
       <c r="J27" t="n">
-        <v>40.37392663955688</v>
+        <v>40.03529286384583</v>
       </c>
     </row>
     <row r="28">
@@ -1309,31 +1309,31 @@
         <v>205</v>
       </c>
       <c r="B28" t="n">
-        <v>2632</v>
+        <v>2636</v>
       </c>
       <c r="C28" t="n">
         <v>2656</v>
       </c>
       <c r="D28" t="n">
-        <v>2631</v>
+        <v>2635</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G28" t="n">
-        <v>99.09604519774011</v>
+        <v>99.24670433145009</v>
       </c>
       <c r="H28" t="n">
         <v>100</v>
       </c>
       <c r="I28" t="n">
-        <v>0.009036144578313253</v>
+        <v>0.007530120481927711</v>
       </c>
       <c r="J28" t="n">
-        <v>42.4861798286438</v>
+        <v>39.17910933494568</v>
       </c>
     </row>
     <row r="29">
@@ -1341,31 +1341,31 @@
         <v>207</v>
       </c>
       <c r="B29" t="n">
-        <v>2077</v>
+        <v>2080</v>
       </c>
       <c r="C29" t="n">
         <v>1859</v>
       </c>
       <c r="D29" t="n">
-        <v>1850</v>
+        <v>1853</v>
       </c>
       <c r="E29" t="n">
         <v>226</v>
       </c>
       <c r="F29" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G29" t="n">
-        <v>99.56942949407966</v>
+        <v>99.73089343379978</v>
       </c>
       <c r="H29" t="n">
-        <v>89.11368015414259</v>
+        <v>89.12938912938912</v>
       </c>
       <c r="I29" t="n">
-        <v>0.1258741258741259</v>
+        <v>0.1242603550295858</v>
       </c>
       <c r="J29" t="n">
-        <v>43.010826587677</v>
+        <v>39.04643154144287</v>
       </c>
     </row>
     <row r="30">
@@ -1373,31 +1373,31 @@
         <v>208</v>
       </c>
       <c r="B30" t="n">
-        <v>2941</v>
+        <v>2946</v>
       </c>
       <c r="C30" t="n">
         <v>2953</v>
       </c>
       <c r="D30" t="n">
-        <v>2934</v>
+        <v>2938</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F30" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G30" t="n">
-        <v>99.39024390243902</v>
+        <v>99.52574525745257</v>
       </c>
       <c r="H30" t="n">
-        <v>99.79591836734694</v>
+        <v>99.7623089983022</v>
       </c>
       <c r="I30" t="n">
-        <v>0.008127328140873687</v>
+        <v>0.007111412123264477</v>
       </c>
       <c r="J30" t="n">
-        <v>41.79293942451477</v>
+        <v>39.92961001396179</v>
       </c>
     </row>
     <row r="31">
@@ -1405,31 +1405,31 @@
         <v>209</v>
       </c>
       <c r="B31" t="n">
-        <v>3000</v>
+        <v>3004</v>
       </c>
       <c r="C31" t="n">
         <v>3004</v>
       </c>
       <c r="D31" t="n">
-        <v>2999</v>
+        <v>3003</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>99.86679986679987</v>
+        <v>100</v>
       </c>
       <c r="H31" t="n">
         <v>100</v>
       </c>
       <c r="I31" t="n">
-        <v>0.001331557922769641</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>41.66119456291199</v>
+        <v>40.67114925384521</v>
       </c>
     </row>
     <row r="32">
@@ -1437,31 +1437,31 @@
         <v>210</v>
       </c>
       <c r="B32" t="n">
-        <v>2626</v>
+        <v>2631</v>
       </c>
       <c r="C32" t="n">
         <v>2649</v>
       </c>
       <c r="D32" t="n">
-        <v>2623</v>
+        <v>2628</v>
       </c>
       <c r="E32" t="n">
         <v>2</v>
       </c>
       <c r="F32" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G32" t="n">
-        <v>99.0558912386707</v>
+        <v>99.24471299093656</v>
       </c>
       <c r="H32" t="n">
-        <v>99.92380952380952</v>
+        <v>99.92395437262357</v>
       </c>
       <c r="I32" t="n">
-        <v>0.0101925254813137</v>
+        <v>0.008305020762551907</v>
       </c>
       <c r="J32" t="n">
-        <v>39.86993980407715</v>
+        <v>38.66800832748413</v>
       </c>
     </row>
     <row r="33">
@@ -1469,31 +1469,31 @@
         <v>212</v>
       </c>
       <c r="B33" t="n">
-        <v>2744</v>
+        <v>2748</v>
       </c>
       <c r="C33" t="n">
         <v>2747</v>
       </c>
       <c r="D33" t="n">
-        <v>2742</v>
+        <v>2746</v>
       </c>
       <c r="E33" t="n">
         <v>1</v>
       </c>
       <c r="F33" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>99.8543335761107</v>
+        <v>100</v>
       </c>
       <c r="H33" t="n">
-        <v>99.96354356543929</v>
+        <v>99.96359665089189</v>
       </c>
       <c r="I33" t="n">
-        <v>0.001820167455405897</v>
+        <v>0.0003640334910811795</v>
       </c>
       <c r="J33" t="n">
-        <v>41.87754821777344</v>
+        <v>41.30889797210693</v>
       </c>
     </row>
     <row r="34">
@@ -1501,31 +1501,31 @@
         <v>213</v>
       </c>
       <c r="B34" t="n">
-        <v>3241</v>
+        <v>3246</v>
       </c>
       <c r="C34" t="n">
         <v>3248</v>
       </c>
       <c r="D34" t="n">
-        <v>3240</v>
+        <v>3243</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G34" t="n">
-        <v>99.78441638435478</v>
+        <v>99.87680936248844</v>
       </c>
       <c r="H34" t="n">
-        <v>100</v>
+        <v>99.93836671802774</v>
       </c>
       <c r="I34" t="n">
-        <v>0.002155172413793103</v>
+        <v>0.001847290640394089</v>
       </c>
       <c r="J34" t="n">
-        <v>42.98872852325439</v>
+        <v>42.45559024810791</v>
       </c>
     </row>
     <row r="35">
@@ -1533,31 +1533,31 @@
         <v>214</v>
       </c>
       <c r="B35" t="n">
-        <v>2257</v>
+        <v>2260</v>
       </c>
       <c r="C35" t="n">
         <v>2261</v>
       </c>
       <c r="D35" t="n">
-        <v>2254</v>
+        <v>2257</v>
       </c>
       <c r="E35" t="n">
         <v>2</v>
       </c>
       <c r="F35" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G35" t="n">
-        <v>99.73451327433628</v>
+        <v>99.86725663716814</v>
       </c>
       <c r="H35" t="n">
-        <v>99.91134751773049</v>
+        <v>99.91146525011067</v>
       </c>
       <c r="I35" t="n">
-        <v>0.003538257408226449</v>
+        <v>0.00221141088014153</v>
       </c>
       <c r="J35" t="n">
-        <v>39.72264122962952</v>
+        <v>38.81683039665222</v>
       </c>
     </row>
     <row r="36">
@@ -1565,31 +1565,31 @@
         <v>215</v>
       </c>
       <c r="B36" t="n">
-        <v>3355</v>
+        <v>3360</v>
       </c>
       <c r="C36" t="n">
         <v>3361</v>
       </c>
       <c r="D36" t="n">
-        <v>3354</v>
+        <v>3358</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G36" t="n">
-        <v>99.82142857142857</v>
+        <v>99.94047619047619</v>
       </c>
       <c r="H36" t="n">
-        <v>100</v>
+        <v>99.97022923489133</v>
       </c>
       <c r="I36" t="n">
-        <v>0.001785182981255579</v>
+        <v>0.0008925914906277894</v>
       </c>
       <c r="J36" t="n">
-        <v>41.08710694313049</v>
+        <v>40.56647419929504</v>
       </c>
     </row>
     <row r="37">
@@ -1597,31 +1597,31 @@
         <v>217</v>
       </c>
       <c r="B37" t="n">
-        <v>2238</v>
+        <v>2244</v>
       </c>
       <c r="C37" t="n">
         <v>2207</v>
       </c>
       <c r="D37" t="n">
-        <v>2200</v>
+        <v>2203</v>
       </c>
       <c r="E37" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F37" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G37" t="n">
-        <v>99.72801450589301</v>
+        <v>99.86400725294651</v>
       </c>
       <c r="H37" t="n">
-        <v>98.34599910594547</v>
+        <v>98.21667409719126</v>
       </c>
       <c r="I37" t="n">
         <v>0.01948346171273221</v>
       </c>
       <c r="J37" t="n">
-        <v>40.09061789512634</v>
+        <v>39.83054828643799</v>
       </c>
     </row>
     <row r="38">
@@ -1629,31 +1629,31 @@
         <v>219</v>
       </c>
       <c r="B38" t="n">
-        <v>2150</v>
+        <v>2154</v>
       </c>
       <c r="C38" t="n">
         <v>2154</v>
       </c>
       <c r="D38" t="n">
-        <v>2149</v>
+        <v>2153</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>99.81421272642824</v>
+        <v>100</v>
       </c>
       <c r="H38" t="n">
         <v>100</v>
       </c>
       <c r="I38" t="n">
-        <v>0.001857010213556175</v>
+        <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>39.56079149246216</v>
+        <v>38.70576238632202</v>
       </c>
     </row>
     <row r="39">
@@ -1661,31 +1661,31 @@
         <v>220</v>
       </c>
       <c r="B39" t="n">
-        <v>2044</v>
+        <v>2048</v>
       </c>
       <c r="C39" t="n">
         <v>2047</v>
       </c>
       <c r="D39" t="n">
-        <v>2043</v>
+        <v>2046</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>99.8533724340176</v>
+        <v>100</v>
       </c>
       <c r="H39" t="n">
-        <v>100</v>
+        <v>99.95114802149487</v>
       </c>
       <c r="I39" t="n">
-        <v>0.001465559355153884</v>
+        <v>0.0004885197850512946</v>
       </c>
       <c r="J39" t="n">
-        <v>39.70049619674683</v>
+        <v>39.44895362854004</v>
       </c>
     </row>
     <row r="40">
@@ -1693,31 +1693,31 @@
         <v>221</v>
       </c>
       <c r="B40" t="n">
-        <v>2420</v>
+        <v>2423</v>
       </c>
       <c r="C40" t="n">
         <v>2427</v>
       </c>
       <c r="D40" t="n">
-        <v>2417</v>
+        <v>2420</v>
       </c>
       <c r="E40" t="n">
         <v>2</v>
       </c>
       <c r="F40" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G40" t="n">
-        <v>99.6290189612531</v>
+        <v>99.75267930750206</v>
       </c>
       <c r="H40" t="n">
-        <v>99.91732120711038</v>
+        <v>99.91742361684558</v>
       </c>
       <c r="I40" t="n">
-        <v>0.004532344458178822</v>
+        <v>0.003296250515039143</v>
       </c>
       <c r="J40" t="n">
-        <v>39.07916498184204</v>
+        <v>38.75133562088013</v>
       </c>
     </row>
     <row r="41">
@@ -1725,31 +1725,31 @@
         <v>222</v>
       </c>
       <c r="B41" t="n">
-        <v>2482</v>
+        <v>2485</v>
       </c>
       <c r="C41" t="n">
         <v>2482</v>
       </c>
       <c r="D41" t="n">
-        <v>2477</v>
+        <v>2480</v>
       </c>
       <c r="E41" t="n">
         <v>4</v>
       </c>
       <c r="F41" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G41" t="n">
-        <v>99.83877468762596</v>
+        <v>99.95969367190649</v>
       </c>
       <c r="H41" t="n">
-        <v>99.83877468762596</v>
+        <v>99.8389694041868</v>
       </c>
       <c r="I41" t="n">
-        <v>0.0032232070910556</v>
+        <v>0.00201450443190975</v>
       </c>
       <c r="J41" t="n">
-        <v>40.2269492149353</v>
+        <v>39.67737984657288</v>
       </c>
     </row>
     <row r="42">
@@ -1757,31 +1757,31 @@
         <v>223</v>
       </c>
       <c r="B42" t="n">
-        <v>2592</v>
+        <v>2595</v>
       </c>
       <c r="C42" t="n">
         <v>2605</v>
       </c>
       <c r="D42" t="n">
-        <v>2590</v>
+        <v>2593</v>
       </c>
       <c r="E42" t="n">
         <v>1</v>
       </c>
       <c r="F42" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G42" t="n">
-        <v>99.46236559139786</v>
+        <v>99.57757296466974</v>
       </c>
       <c r="H42" t="n">
-        <v>99.96140486298727</v>
+        <v>99.96144949884348</v>
       </c>
       <c r="I42" t="n">
-        <v>0.005758157389635317</v>
+        <v>0.004606525911708253</v>
       </c>
       <c r="J42" t="n">
-        <v>39.86513805389404</v>
+        <v>39.69928050041199</v>
       </c>
     </row>
     <row r="43">
@@ -1789,31 +1789,31 @@
         <v>228</v>
       </c>
       <c r="B43" t="n">
-        <v>2059</v>
+        <v>2062</v>
       </c>
       <c r="C43" t="n">
         <v>2052</v>
       </c>
       <c r="D43" t="n">
-        <v>2040</v>
+        <v>2043</v>
       </c>
       <c r="E43" t="n">
         <v>18</v>
       </c>
       <c r="F43" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G43" t="n">
-        <v>99.46367625548513</v>
+        <v>99.60994636762555</v>
       </c>
       <c r="H43" t="n">
-        <v>99.12536443148689</v>
+        <v>99.12663755458516</v>
       </c>
       <c r="I43" t="n">
-        <v>0.01413255360623782</v>
+        <v>0.01267056530214425</v>
       </c>
       <c r="J43" t="n">
-        <v>40.17763328552246</v>
+        <v>39.53414726257324</v>
       </c>
     </row>
     <row r="44">
@@ -1821,31 +1821,31 @@
         <v>230</v>
       </c>
       <c r="B44" t="n">
-        <v>2251</v>
+        <v>2255</v>
       </c>
       <c r="C44" t="n">
         <v>2255</v>
       </c>
       <c r="D44" t="n">
-        <v>2250</v>
+        <v>2254</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>99.82253771073647</v>
+        <v>100</v>
       </c>
       <c r="H44" t="n">
         <v>100</v>
       </c>
       <c r="I44" t="n">
-        <v>0.001773835920177384</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>40.1376416683197</v>
+        <v>39.54850363731384</v>
       </c>
     </row>
     <row r="45">
@@ -1853,31 +1853,31 @@
         <v>231</v>
       </c>
       <c r="B45" t="n">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="C45" t="n">
         <v>1570</v>
       </c>
       <c r="D45" t="n">
-        <v>1567</v>
+        <v>1569</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>99.87253027405991</v>
+        <v>100</v>
       </c>
       <c r="H45" t="n">
-        <v>99.87253027405991</v>
+        <v>99.93630573248407</v>
       </c>
       <c r="I45" t="n">
-        <v>0.002547770700636943</v>
+        <v>0.0006369426751592356</v>
       </c>
       <c r="J45" t="n">
-        <v>39.1861138343811</v>
+        <v>39.11789321899414</v>
       </c>
     </row>
     <row r="46">
@@ -1885,31 +1885,31 @@
         <v>232</v>
       </c>
       <c r="B46" t="n">
-        <v>1786</v>
+        <v>1788</v>
       </c>
       <c r="C46" t="n">
         <v>1780</v>
       </c>
       <c r="D46" t="n">
-        <v>1776</v>
+        <v>1779</v>
       </c>
       <c r="E46" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F46" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>99.83136593591905</v>
+        <v>100</v>
       </c>
       <c r="H46" t="n">
-        <v>99.49579831932773</v>
+        <v>99.55232232792389</v>
       </c>
       <c r="I46" t="n">
-        <v>0.006741573033707865</v>
+        <v>0.004494382022471911</v>
       </c>
       <c r="J46" t="n">
-        <v>39.64963030815125</v>
+        <v>38.98607730865479</v>
       </c>
     </row>
     <row r="47">
@@ -1917,31 +1917,31 @@
         <v>233</v>
       </c>
       <c r="B47" t="n">
-        <v>3073</v>
+        <v>3078</v>
       </c>
       <c r="C47" t="n">
         <v>3077</v>
       </c>
       <c r="D47" t="n">
-        <v>3072</v>
+        <v>3076</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>99.86996098829648</v>
+        <v>100</v>
       </c>
       <c r="H47" t="n">
-        <v>100</v>
+        <v>99.96750081247968</v>
       </c>
       <c r="I47" t="n">
-        <v>0.00129996750081248</v>
+        <v>0.0003249918752031199</v>
       </c>
       <c r="J47" t="n">
-        <v>41.35121560096741</v>
+        <v>40.61768221855164</v>
       </c>
     </row>
     <row r="48">
@@ -1949,31 +1949,31 @@
         <v>234</v>
       </c>
       <c r="B48" t="n">
-        <v>2748</v>
+        <v>2752</v>
       </c>
       <c r="C48" t="n">
         <v>2752</v>
       </c>
       <c r="D48" t="n">
-        <v>2747</v>
+        <v>2751</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>99.85459832788077</v>
+        <v>100</v>
       </c>
       <c r="H48" t="n">
         <v>100</v>
       </c>
       <c r="I48" t="n">
-        <v>0.001453488372093023</v>
+        <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>39.86488199234009</v>
+        <v>39.41820311546326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing the parameters for locate r_prak function
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/attempt1.xlsx
+++ b/R peak detection/beatdetection/attempt1.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="agsuy" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>37.63093018531799</v>
+        <v>35.66036176681519</v>
       </c>
     </row>
     <row r="2">
@@ -501,7 +501,7 @@
         <v>0.000536480686695279</v>
       </c>
       <c r="J2" t="n">
-        <v>38.19485068321228</v>
+        <v>35.27510190010071</v>
       </c>
     </row>
     <row r="3">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>38.67928028106689</v>
+        <v>35.63436627388</v>
       </c>
     </row>
     <row r="4">
@@ -565,7 +565,7 @@
         <v>0.0004798464491362764</v>
       </c>
       <c r="J4" t="n">
-        <v>39.04195380210876</v>
+        <v>35.85895705223083</v>
       </c>
     </row>
     <row r="5">
@@ -597,7 +597,7 @@
         <v>0.008527827648114902</v>
       </c>
       <c r="J5" t="n">
-        <v>39.25133323669434</v>
+        <v>36.01353073120117</v>
       </c>
     </row>
     <row r="6">
@@ -629,7 +629,7 @@
         <v>0.01050175029171529</v>
       </c>
       <c r="J6" t="n">
-        <v>39.79677248001099</v>
+        <v>36.64841961860657</v>
       </c>
     </row>
     <row r="7">
@@ -661,7 +661,7 @@
         <v>0.001480019733596448</v>
       </c>
       <c r="J7" t="n">
-        <v>39.46328949928284</v>
+        <v>36.25137758255005</v>
       </c>
     </row>
     <row r="8">
@@ -693,7 +693,7 @@
         <v>0.01358313817330211</v>
       </c>
       <c r="J8" t="n">
-        <v>40.28286266326904</v>
+        <v>36.87122178077698</v>
       </c>
     </row>
     <row r="9">
@@ -725,7 +725,7 @@
         <v>0.03178206583427923</v>
       </c>
       <c r="J9" t="n">
-        <v>39.54617071151733</v>
+        <v>35.86889672279358</v>
       </c>
     </row>
     <row r="10">
@@ -757,7 +757,7 @@
         <v>0.002766798418972332</v>
       </c>
       <c r="J10" t="n">
-        <v>39.61692547798157</v>
+        <v>36.32108521461487</v>
       </c>
     </row>
     <row r="11">
@@ -789,7 +789,7 @@
         <v>0.002354048964218456</v>
       </c>
       <c r="J11" t="n">
-        <v>39.57951736450195</v>
+        <v>36.12348079681396</v>
       </c>
     </row>
     <row r="12">
@@ -821,7 +821,7 @@
         <v>0.003152088258471237</v>
       </c>
       <c r="J12" t="n">
-        <v>39.15743851661682</v>
+        <v>36.08053636550903</v>
       </c>
     </row>
     <row r="13">
@@ -853,7 +853,7 @@
         <v>0.001114827201783724</v>
       </c>
       <c r="J13" t="n">
-        <v>39.72747802734375</v>
+        <v>35.7022557258606</v>
       </c>
     </row>
     <row r="14">
@@ -885,7 +885,7 @@
         <v>0.006386375731772219</v>
       </c>
       <c r="J14" t="n">
-        <v>38.87654781341553</v>
+        <v>35.80611824989319</v>
       </c>
     </row>
     <row r="15">
@@ -917,7 +917,7 @@
         <v>0.0005120327700972862</v>
       </c>
       <c r="J15" t="n">
-        <v>38.48779344558716</v>
+        <v>35.24312305450439</v>
       </c>
     </row>
     <row r="16">
@@ -949,7 +949,7 @@
         <v>0.009954375777685608</v>
       </c>
       <c r="J16" t="n">
-        <v>40.73249101638794</v>
+        <v>36.49177050590515</v>
       </c>
     </row>
     <row r="17">
@@ -981,7 +981,7 @@
         <v>0.000651890482398957</v>
       </c>
       <c r="J17" t="n">
-        <v>39.60176634788513</v>
+        <v>36.28306865692139</v>
       </c>
     </row>
     <row r="18">
@@ -1013,7 +1013,7 @@
         <v>0.002196836555360281</v>
       </c>
       <c r="J18" t="n">
-        <v>41.20593619346619</v>
+        <v>37.03895664215088</v>
       </c>
     </row>
     <row r="19">
@@ -1045,7 +1045,7 @@
         <v>0.001509813789632612</v>
       </c>
       <c r="J19" t="n">
-        <v>42.99114060401917</v>
+        <v>35.94142127037048</v>
       </c>
     </row>
     <row r="20">
@@ -1077,7 +1077,7 @@
         <v>0.001073537305421363</v>
       </c>
       <c r="J20" t="n">
-        <v>38.84943127632141</v>
+        <v>35.18150424957275</v>
       </c>
     </row>
     <row r="21">
@@ -1109,7 +1109,7 @@
         <v>0.0004042037186742118</v>
       </c>
       <c r="J21" t="n">
-        <v>39.91568899154663</v>
+        <v>36.30312657356262</v>
       </c>
     </row>
     <row r="22">
@@ -1141,7 +1141,7 @@
         <v>0.001318391562294001</v>
       </c>
       <c r="J22" t="n">
-        <v>39.1142258644104</v>
+        <v>35.24853181838989</v>
       </c>
     </row>
     <row r="23">
@@ -1173,7 +1173,7 @@
         <v>0.001235330450895615</v>
       </c>
       <c r="J23" t="n">
-        <v>39.34931707382202</v>
+        <v>35.65342211723328</v>
       </c>
     </row>
     <row r="24">
@@ -1205,7 +1205,7 @@
         <v>0.003846153846153846</v>
       </c>
       <c r="J24" t="n">
-        <v>40.02467513084412</v>
+        <v>36.1482834815979</v>
       </c>
     </row>
     <row r="25">
@@ -1237,7 +1237,7 @@
         <v>0.006622516556291391</v>
       </c>
       <c r="J25" t="n">
-        <v>38.52096438407898</v>
+        <v>35.22927808761597</v>
       </c>
     </row>
     <row r="26">
@@ -1269,7 +1269,7 @@
         <v>0.005149812734082397</v>
       </c>
       <c r="J26" t="n">
-        <v>38.76453590393066</v>
+        <v>35.49432039260864</v>
       </c>
     </row>
     <row r="27">
@@ -1301,7 +1301,7 @@
         <v>0.03258313738663084</v>
       </c>
       <c r="J27" t="n">
-        <v>40.03529286384583</v>
+        <v>36.83135080337524</v>
       </c>
     </row>
     <row r="28">
@@ -1333,7 +1333,7 @@
         <v>0.007530120481927711</v>
       </c>
       <c r="J28" t="n">
-        <v>39.17910933494568</v>
+        <v>35.55908012390137</v>
       </c>
     </row>
     <row r="29">
@@ -1365,7 +1365,7 @@
         <v>0.1242603550295858</v>
       </c>
       <c r="J29" t="n">
-        <v>39.04643154144287</v>
+        <v>35.77238821983337</v>
       </c>
     </row>
     <row r="30">
@@ -1397,7 +1397,7 @@
         <v>0.007111412123264477</v>
       </c>
       <c r="J30" t="n">
-        <v>39.92961001396179</v>
+        <v>36.59109735488892</v>
       </c>
     </row>
     <row r="31">
@@ -1429,7 +1429,7 @@
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>40.67114925384521</v>
+        <v>36.44655609130859</v>
       </c>
     </row>
     <row r="32">
@@ -1461,7 +1461,7 @@
         <v>0.008305020762551907</v>
       </c>
       <c r="J32" t="n">
-        <v>38.66800832748413</v>
+        <v>35.42531585693359</v>
       </c>
     </row>
     <row r="33">
@@ -1493,7 +1493,7 @@
         <v>0.0003640334910811795</v>
       </c>
       <c r="J33" t="n">
-        <v>41.30889797210693</v>
+        <v>37.54795575141907</v>
       </c>
     </row>
     <row r="34">
@@ -1525,7 +1525,7 @@
         <v>0.001847290640394089</v>
       </c>
       <c r="J34" t="n">
-        <v>42.45559024810791</v>
+        <v>38.58660840988159</v>
       </c>
     </row>
     <row r="35">
@@ -1557,7 +1557,7 @@
         <v>0.00221141088014153</v>
       </c>
       <c r="J35" t="n">
-        <v>38.81683039665222</v>
+        <v>35.66844010353088</v>
       </c>
     </row>
     <row r="36">
@@ -1589,7 +1589,7 @@
         <v>0.0008925914906277894</v>
       </c>
       <c r="J36" t="n">
-        <v>40.56647419929504</v>
+        <v>36.98784446716309</v>
       </c>
     </row>
     <row r="37">
@@ -1621,7 +1621,7 @@
         <v>0.01948346171273221</v>
       </c>
       <c r="J37" t="n">
-        <v>39.83054828643799</v>
+        <v>36.35196089744568</v>
       </c>
     </row>
     <row r="38">
@@ -1653,7 +1653,7 @@
         <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>38.70576238632202</v>
+        <v>37.52797031402588</v>
       </c>
     </row>
     <row r="39">
@@ -1685,7 +1685,7 @@
         <v>0.0004885197850512946</v>
       </c>
       <c r="J39" t="n">
-        <v>39.44895362854004</v>
+        <v>36.07941365242004</v>
       </c>
     </row>
     <row r="40">
@@ -1717,7 +1717,7 @@
         <v>0.003296250515039143</v>
       </c>
       <c r="J40" t="n">
-        <v>38.75133562088013</v>
+        <v>35.14920425415039</v>
       </c>
     </row>
     <row r="41">
@@ -1749,7 +1749,7 @@
         <v>0.00201450443190975</v>
       </c>
       <c r="J41" t="n">
-        <v>39.67737984657288</v>
+        <v>35.61071491241455</v>
       </c>
     </row>
     <row r="42">
@@ -1781,7 +1781,7 @@
         <v>0.004606525911708253</v>
       </c>
       <c r="J42" t="n">
-        <v>39.69928050041199</v>
+        <v>35.67176651954651</v>
       </c>
     </row>
     <row r="43">
@@ -1813,7 +1813,7 @@
         <v>0.01267056530214425</v>
       </c>
       <c r="J43" t="n">
-        <v>39.53414726257324</v>
+        <v>35.98828673362732</v>
       </c>
     </row>
     <row r="44">
@@ -1845,7 +1845,7 @@
         <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>39.54850363731384</v>
+        <v>36.20944476127625</v>
       </c>
     </row>
     <row r="45">
@@ -1877,7 +1877,7 @@
         <v>0.0006369426751592356</v>
       </c>
       <c r="J45" t="n">
-        <v>39.11789321899414</v>
+        <v>35.7984356880188</v>
       </c>
     </row>
     <row r="46">
@@ -1909,7 +1909,7 @@
         <v>0.004494382022471911</v>
       </c>
       <c r="J46" t="n">
-        <v>38.98607730865479</v>
+        <v>35.46314167976379</v>
       </c>
     </row>
     <row r="47">
@@ -1941,7 +1941,7 @@
         <v>0.0003249918752031199</v>
       </c>
       <c r="J47" t="n">
-        <v>40.61768221855164</v>
+        <v>36.8673210144043</v>
       </c>
     </row>
     <row r="48">
@@ -1973,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>39.41820311546326</v>
+        <v>35.98003172874451</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing c to 3.25
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/attempt1.xlsx
+++ b/R peak detection/beatdetection/attempt1.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="stfiulok" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="jhagjas" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>38.99940824508667</v>
+        <v>38.54852271080017</v>
       </c>
     </row>
     <row r="2">
@@ -501,7 +501,7 @@
         <v>0.000536480686695279</v>
       </c>
       <c r="J2" t="n">
-        <v>39.87541532516479</v>
+        <v>39.10971736907959</v>
       </c>
     </row>
     <row r="3">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>39.63791823387146</v>
+        <v>39.3399076461792</v>
       </c>
     </row>
     <row r="4">
@@ -565,7 +565,7 @@
         <v>0.0004798464491362764</v>
       </c>
       <c r="J4" t="n">
-        <v>39.83335757255554</v>
+        <v>39.47608399391174</v>
       </c>
     </row>
     <row r="5">
@@ -597,7 +597,7 @@
         <v>0.005385996409335727</v>
       </c>
       <c r="J5" t="n">
-        <v>40.29621529579163</v>
+        <v>39.79212856292725</v>
       </c>
     </row>
     <row r="6">
@@ -605,31 +605,31 @@
         <v>105</v>
       </c>
       <c r="B6" t="n">
-        <v>2581</v>
+        <v>2578</v>
       </c>
       <c r="C6" t="n">
         <v>2571</v>
       </c>
       <c r="D6" t="n">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="E6" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F6" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G6" t="n">
-        <v>99.53307392996109</v>
+        <v>99.49416342412451</v>
       </c>
       <c r="H6" t="n">
-        <v>99.14728682170542</v>
+        <v>99.22390376406675</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0132244262932711</v>
+        <v>0.01283547257876313</v>
       </c>
       <c r="J6" t="n">
-        <v>40.54922866821289</v>
+        <v>40.30218744277954</v>
       </c>
     </row>
     <row r="7">
@@ -661,7 +661,7 @@
         <v>0.001973359644795264</v>
       </c>
       <c r="J7" t="n">
-        <v>40.35662460327148</v>
+        <v>40.1474404335022</v>
       </c>
     </row>
     <row r="8">
@@ -669,7 +669,7 @@
         <v>107</v>
       </c>
       <c r="B8" t="n">
-        <v>2247</v>
+        <v>2181</v>
       </c>
       <c r="C8" t="n">
         <v>2135</v>
@@ -678,7 +678,7 @@
         <v>2133</v>
       </c>
       <c r="E8" t="n">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -687,13 +687,13 @@
         <v>99.95313964386129</v>
       </c>
       <c r="H8" t="n">
-        <v>94.96883348174532</v>
+        <v>97.8440366972477</v>
       </c>
       <c r="I8" t="n">
-        <v>0.05339578454332553</v>
+        <v>0.0224824355971897</v>
       </c>
       <c r="J8" t="n">
-        <v>40.78594398498535</v>
+        <v>40.87517118453979</v>
       </c>
     </row>
     <row r="9">
@@ -701,7 +701,7 @@
         <v>108</v>
       </c>
       <c r="B9" t="n">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="C9" t="n">
         <v>1762</v>
@@ -710,7 +710,7 @@
         <v>1754</v>
       </c>
       <c r="E9" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9" t="n">
         <v>7</v>
@@ -719,13 +719,13 @@
         <v>99.60249858035208</v>
       </c>
       <c r="H9" t="n">
-        <v>99.2081447963801</v>
+        <v>99.26428975664969</v>
       </c>
       <c r="I9" t="n">
-        <v>0.01191827468785471</v>
+        <v>0.01135073779795687</v>
       </c>
       <c r="J9" t="n">
-        <v>39.86619853973389</v>
+        <v>39.79865431785583</v>
       </c>
     </row>
     <row r="10">
@@ -757,7 +757,7 @@
         <v>0.002370604504148558</v>
       </c>
       <c r="J10" t="n">
-        <v>40.17154407501221</v>
+        <v>40.04406905174255</v>
       </c>
     </row>
     <row r="11">
@@ -789,7 +789,7 @@
         <v>0.001883239171374765</v>
       </c>
       <c r="J11" t="n">
-        <v>40.4782087802887</v>
+        <v>40.00422048568726</v>
       </c>
     </row>
     <row r="12">
@@ -797,7 +797,7 @@
         <v>112</v>
       </c>
       <c r="B12" t="n">
-        <v>2541</v>
+        <v>2539</v>
       </c>
       <c r="C12" t="n">
         <v>2538</v>
@@ -806,7 +806,7 @@
         <v>2537</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -815,13 +815,13 @@
         <v>100</v>
       </c>
       <c r="H12" t="n">
-        <v>99.88188976377953</v>
+        <v>99.96059889676911</v>
       </c>
       <c r="I12" t="n">
-        <v>0.001182033096926714</v>
+        <v>0.0003940110323089047</v>
       </c>
       <c r="J12" t="n">
-        <v>39.78483366966248</v>
+        <v>39.75757908821106</v>
       </c>
     </row>
     <row r="13">
@@ -829,7 +829,7 @@
         <v>113</v>
       </c>
       <c r="B13" t="n">
-        <v>1812</v>
+        <v>1806</v>
       </c>
       <c r="C13" t="n">
         <v>1795</v>
@@ -838,7 +838,7 @@
         <v>1793</v>
       </c>
       <c r="E13" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -847,13 +847,13 @@
         <v>99.94425863991081</v>
       </c>
       <c r="H13" t="n">
-        <v>99.00607399226946</v>
+        <v>99.33518005540166</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0105849582172702</v>
+        <v>0.007242339832869081</v>
       </c>
       <c r="J13" t="n">
-        <v>40.13408899307251</v>
+        <v>39.88439130783081</v>
       </c>
     </row>
     <row r="14">
@@ -885,7 +885,7 @@
         <v>0.006386375731772219</v>
       </c>
       <c r="J14" t="n">
-        <v>39.70046663284302</v>
+        <v>39.70295524597168</v>
       </c>
     </row>
     <row r="15">
@@ -917,7 +917,7 @@
         <v>0.0005120327700972862</v>
       </c>
       <c r="J15" t="n">
-        <v>39.18021702766418</v>
+        <v>39.24021124839783</v>
       </c>
     </row>
     <row r="16">
@@ -949,7 +949,7 @@
         <v>0.009954375777685608</v>
       </c>
       <c r="J16" t="n">
-        <v>40.85026431083679</v>
+        <v>40.54644918441772</v>
       </c>
     </row>
     <row r="17">
@@ -957,7 +957,7 @@
         <v>117</v>
       </c>
       <c r="B17" t="n">
-        <v>1538</v>
+        <v>1534</v>
       </c>
       <c r="C17" t="n">
         <v>1534</v>
@@ -966,7 +966,7 @@
         <v>1533</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -975,13 +975,13 @@
         <v>100</v>
       </c>
       <c r="H17" t="n">
-        <v>99.73975276512687</v>
+        <v>100</v>
       </c>
       <c r="I17" t="n">
-        <v>0.002607561929595828</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>39.90968656539917</v>
+        <v>39.79909944534302</v>
       </c>
     </row>
     <row r="18">
@@ -1013,7 +1013,7 @@
         <v>0.002196836555360281</v>
       </c>
       <c r="J18" t="n">
-        <v>40.92570352554321</v>
+        <v>40.52464532852173</v>
       </c>
     </row>
     <row r="19">
@@ -1045,7 +1045,7 @@
         <v>0.002516356316054353</v>
       </c>
       <c r="J19" t="n">
-        <v>40.28345108032227</v>
+        <v>42.02813577651978</v>
       </c>
     </row>
     <row r="20">
@@ -1077,7 +1077,7 @@
         <v>0.001610305958132045</v>
       </c>
       <c r="J20" t="n">
-        <v>39.79833626747131</v>
+        <v>39.72353029251099</v>
       </c>
     </row>
     <row r="21">
@@ -1109,7 +1109,7 @@
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>40.19138789176941</v>
+        <v>40.10713529586792</v>
       </c>
     </row>
     <row r="22">
@@ -1117,7 +1117,7 @@
         <v>123</v>
       </c>
       <c r="B22" t="n">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="C22" t="n">
         <v>1517</v>
@@ -1126,7 +1126,7 @@
         <v>1516</v>
       </c>
       <c r="E22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1135,13 +1135,13 @@
         <v>100</v>
       </c>
       <c r="H22" t="n">
-        <v>99.80250164581962</v>
+        <v>99.86824769433466</v>
       </c>
       <c r="I22" t="n">
-        <v>0.001977587343441002</v>
+        <v>0.001318391562294001</v>
       </c>
       <c r="J22" t="n">
-        <v>39.82651591300964</v>
+        <v>39.75511240959167</v>
       </c>
     </row>
     <row r="23">
@@ -1173,7 +1173,7 @@
         <v>0.001235330450895615</v>
       </c>
       <c r="J23" t="n">
-        <v>39.38858127593994</v>
+        <v>39.36995577812195</v>
       </c>
     </row>
     <row r="24">
@@ -1205,7 +1205,7 @@
         <v>0.001537870049980777</v>
       </c>
       <c r="J24" t="n">
-        <v>40.28170418739319</v>
+        <v>40.043301820755</v>
       </c>
     </row>
     <row r="25">
@@ -1213,7 +1213,7 @@
         <v>201</v>
       </c>
       <c r="B25" t="n">
-        <v>1957</v>
+        <v>1952</v>
       </c>
       <c r="C25" t="n">
         <v>1963</v>
@@ -1222,7 +1222,7 @@
         <v>1949</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F25" t="n">
         <v>13</v>
@@ -1231,13 +1231,13 @@
         <v>99.33741080530072</v>
       </c>
       <c r="H25" t="n">
-        <v>99.64212678936606</v>
+        <v>99.89748846745259</v>
       </c>
       <c r="I25" t="n">
-        <v>0.01018848700967906</v>
+        <v>0.007641365257259297</v>
       </c>
       <c r="J25" t="n">
-        <v>39.59630703926086</v>
+        <v>39.58996868133545</v>
       </c>
     </row>
     <row r="26">
@@ -1269,7 +1269,7 @@
         <v>0.005149812734082397</v>
       </c>
       <c r="J26" t="n">
-        <v>39.17033767700195</v>
+        <v>39.12427878379822</v>
       </c>
     </row>
     <row r="27">
@@ -1277,31 +1277,31 @@
         <v>203</v>
       </c>
       <c r="B27" t="n">
-        <v>2893</v>
+        <v>2877</v>
       </c>
       <c r="C27" t="n">
         <v>2979</v>
       </c>
       <c r="D27" t="n">
-        <v>2880</v>
+        <v>2864</v>
       </c>
       <c r="E27" t="n">
         <v>12</v>
       </c>
       <c r="F27" t="n">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="G27" t="n">
-        <v>96.70920080591</v>
+        <v>96.1719274680994</v>
       </c>
       <c r="H27" t="n">
-        <v>99.5850622406639</v>
+        <v>99.58275382475661</v>
       </c>
       <c r="I27" t="n">
-        <v>0.03692514266532394</v>
+        <v>0.04229607250755287</v>
       </c>
       <c r="J27" t="n">
-        <v>40.32234334945679</v>
+        <v>40.15285205841064</v>
       </c>
     </row>
     <row r="28">
@@ -1333,7 +1333,7 @@
         <v>0.007530120481927711</v>
       </c>
       <c r="J28" t="n">
-        <v>39.5016074180603</v>
+        <v>39.28722906112671</v>
       </c>
     </row>
     <row r="29">
@@ -1341,31 +1341,31 @@
         <v>207</v>
       </c>
       <c r="B29" t="n">
-        <v>2071</v>
+        <v>2064</v>
       </c>
       <c r="C29" t="n">
         <v>1859</v>
       </c>
       <c r="D29" t="n">
-        <v>1851</v>
+        <v>1852</v>
       </c>
       <c r="E29" t="n">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="F29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G29" t="n">
-        <v>99.62325080731969</v>
+        <v>99.67707212055974</v>
       </c>
       <c r="H29" t="n">
-        <v>89.42028985507247</v>
+        <v>89.77217644207465</v>
       </c>
       <c r="I29" t="n">
-        <v>0.1215707369553523</v>
+        <v>0.1167294244217321</v>
       </c>
       <c r="J29" t="n">
-        <v>39.59423446655273</v>
+        <v>39.38474154472351</v>
       </c>
     </row>
     <row r="30">
@@ -1373,7 +1373,7 @@
         <v>208</v>
       </c>
       <c r="B30" t="n">
-        <v>2945</v>
+        <v>2944</v>
       </c>
       <c r="C30" t="n">
         <v>2953</v>
@@ -1382,7 +1382,7 @@
         <v>2937</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="n">
         <v>15</v>
@@ -1391,13 +1391,13 @@
         <v>99.49186991869918</v>
       </c>
       <c r="H30" t="n">
-        <v>99.76222826086956</v>
+        <v>99.79612640163099</v>
       </c>
       <c r="I30" t="n">
-        <v>0.007450050795800881</v>
+        <v>0.007111412123264477</v>
       </c>
       <c r="J30" t="n">
-        <v>40.25545787811279</v>
+        <v>40.32072949409485</v>
       </c>
     </row>
     <row r="31">
@@ -1429,7 +1429,7 @@
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>40.53528952598572</v>
+        <v>40.25624775886536</v>
       </c>
     </row>
     <row r="32">
@@ -1437,31 +1437,31 @@
         <v>210</v>
       </c>
       <c r="B32" t="n">
-        <v>2625</v>
+        <v>2624</v>
       </c>
       <c r="C32" t="n">
         <v>2649</v>
       </c>
       <c r="D32" t="n">
-        <v>2622</v>
+        <v>2621</v>
       </c>
       <c r="E32" t="n">
         <v>2</v>
       </c>
       <c r="F32" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G32" t="n">
-        <v>99.01812688821752</v>
+        <v>98.98036253776435</v>
       </c>
       <c r="H32" t="n">
-        <v>99.92378048780488</v>
+        <v>99.9237514296607</v>
       </c>
       <c r="I32" t="n">
-        <v>0.01057002642506606</v>
+        <v>0.01094752736881842</v>
       </c>
       <c r="J32" t="n">
-        <v>39.36464071273804</v>
+        <v>39.3378758430481</v>
       </c>
     </row>
     <row r="33">
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>41.2411584854126</v>
+        <v>41.54549169540405</v>
       </c>
     </row>
     <row r="34">
@@ -1501,7 +1501,7 @@
         <v>213</v>
       </c>
       <c r="B34" t="n">
-        <v>3247</v>
+        <v>3246</v>
       </c>
       <c r="C34" t="n">
         <v>3248</v>
@@ -1510,7 +1510,7 @@
         <v>3243</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
         <v>4</v>
@@ -1519,13 +1519,13 @@
         <v>99.87680936248844</v>
       </c>
       <c r="H34" t="n">
-        <v>99.90757855822551</v>
+        <v>99.93836671802774</v>
       </c>
       <c r="I34" t="n">
-        <v>0.002155172413793103</v>
+        <v>0.001847290640394089</v>
       </c>
       <c r="J34" t="n">
-        <v>42.80104207992554</v>
+        <v>43.36691403388977</v>
       </c>
     </row>
     <row r="35">
@@ -1557,7 +1557,7 @@
         <v>0.001326846528084918</v>
       </c>
       <c r="J35" t="n">
-        <v>39.5706570148468</v>
+        <v>39.70415186882019</v>
       </c>
     </row>
     <row r="36">
@@ -1565,31 +1565,31 @@
         <v>215</v>
       </c>
       <c r="B36" t="n">
-        <v>3361</v>
+        <v>3359</v>
       </c>
       <c r="C36" t="n">
         <v>3362</v>
       </c>
       <c r="D36" t="n">
-        <v>3360</v>
+        <v>3358</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G36" t="n">
-        <v>99.9702469503124</v>
+        <v>99.91074085093722</v>
       </c>
       <c r="H36" t="n">
         <v>100</v>
       </c>
       <c r="I36" t="n">
-        <v>0.000297441998810232</v>
+        <v>0.000892325996430696</v>
       </c>
       <c r="J36" t="n">
-        <v>40.91782736778259</v>
+        <v>40.79715967178345</v>
       </c>
     </row>
     <row r="37">
@@ -1597,7 +1597,7 @@
         <v>217</v>
       </c>
       <c r="B37" t="n">
-        <v>3376</v>
+        <v>3282</v>
       </c>
       <c r="C37" t="n">
         <v>2208</v>
@@ -1606,7 +1606,7 @@
         <v>2203</v>
       </c>
       <c r="E37" t="n">
-        <v>1172</v>
+        <v>1078</v>
       </c>
       <c r="F37" t="n">
         <v>4</v>
@@ -1615,13 +1615,13 @@
         <v>99.81875849569552</v>
       </c>
       <c r="H37" t="n">
-        <v>65.27407407407408</v>
+        <v>67.14416336482779</v>
       </c>
       <c r="I37" t="n">
-        <v>0.5326086956521739</v>
+        <v>0.490036231884058</v>
       </c>
       <c r="J37" t="n">
-        <v>40.36697959899902</v>
+        <v>40.4207935333252</v>
       </c>
     </row>
     <row r="38">
@@ -1653,7 +1653,7 @@
         <v>0.0004642525533890436</v>
       </c>
       <c r="J38" t="n">
-        <v>39.45397472381592</v>
+        <v>39.61178946495056</v>
       </c>
     </row>
     <row r="39">
@@ -1685,7 +1685,7 @@
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>39.70100593566895</v>
+        <v>40.35430788993835</v>
       </c>
     </row>
     <row r="40">
@@ -1717,7 +1717,7 @@
         <v>0.002472187886279357</v>
       </c>
       <c r="J40" t="n">
-        <v>39.08483695983887</v>
+        <v>39.30700588226318</v>
       </c>
     </row>
     <row r="41">
@@ -1725,31 +1725,31 @@
         <v>222</v>
       </c>
       <c r="B41" t="n">
-        <v>2486</v>
+        <v>2485</v>
       </c>
       <c r="C41" t="n">
         <v>2482</v>
       </c>
       <c r="D41" t="n">
-        <v>2480</v>
+        <v>2479</v>
       </c>
       <c r="E41" t="n">
         <v>5</v>
       </c>
       <c r="F41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G41" t="n">
-        <v>99.95969367190649</v>
+        <v>99.91938734381299</v>
       </c>
       <c r="H41" t="n">
-        <v>99.79879275653923</v>
+        <v>99.7987117552335</v>
       </c>
       <c r="I41" t="n">
-        <v>0.0024174053182917</v>
+        <v>0.00282030620467365</v>
       </c>
       <c r="J41" t="n">
-        <v>39.47340297698975</v>
+        <v>39.79197692871094</v>
       </c>
     </row>
     <row r="42">
@@ -1781,7 +1781,7 @@
         <v>0.004990403071017275</v>
       </c>
       <c r="J42" t="n">
-        <v>39.75451278686523</v>
+        <v>40.09335041046143</v>
       </c>
     </row>
     <row r="43">
@@ -1789,7 +1789,7 @@
         <v>228</v>
       </c>
       <c r="B43" t="n">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="C43" t="n">
         <v>2052</v>
@@ -1798,7 +1798,7 @@
         <v>2044</v>
       </c>
       <c r="E43" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
         <v>7</v>
@@ -1807,13 +1807,13 @@
         <v>99.65870307167235</v>
       </c>
       <c r="H43" t="n">
-        <v>99.61013645224172</v>
+        <v>99.65870307167235</v>
       </c>
       <c r="I43" t="n">
-        <v>0.007309941520467836</v>
+        <v>0.00682261208576998</v>
       </c>
       <c r="J43" t="n">
-        <v>39.47928953170776</v>
+        <v>39.88975071907043</v>
       </c>
     </row>
     <row r="44">
@@ -1845,7 +1845,7 @@
         <v>0.0004434589800443459</v>
       </c>
       <c r="J44" t="n">
-        <v>39.87569403648376</v>
+        <v>40.35441946983337</v>
       </c>
     </row>
     <row r="45">
@@ -1877,7 +1877,7 @@
         <v>0.001273885350318471</v>
       </c>
       <c r="J45" t="n">
-        <v>39.74608588218689</v>
+        <v>39.83396649360657</v>
       </c>
     </row>
     <row r="46">
@@ -1909,7 +1909,7 @@
         <v>0.002808988764044944</v>
       </c>
       <c r="J46" t="n">
-        <v>39.55425596237183</v>
+        <v>39.27898764610291</v>
       </c>
     </row>
     <row r="47">
@@ -1941,7 +1941,7 @@
         <v>0.0003249918752031199</v>
       </c>
       <c r="J47" t="n">
-        <v>41.59302377700806</v>
+        <v>41.00643682479858</v>
       </c>
     </row>
     <row r="48">
@@ -1973,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>40.27375769615173</v>
+        <v>40.17040872573853</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing window to 0.35 s
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/attempt1.xlsx
+++ b/R peak detection/beatdetection/attempt1.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="jhagjas" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="sdfewf" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>38.54852271080017</v>
+        <v>39.11275243759155</v>
       </c>
     </row>
     <row r="2">
@@ -501,7 +501,7 @@
         <v>0.000536480686695279</v>
       </c>
       <c r="J2" t="n">
-        <v>39.10971736907959</v>
+        <v>38.96059703826904</v>
       </c>
     </row>
     <row r="3">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>39.3399076461792</v>
+        <v>39.64492177963257</v>
       </c>
     </row>
     <row r="4">
@@ -565,7 +565,7 @@
         <v>0.0004798464491362764</v>
       </c>
       <c r="J4" t="n">
-        <v>39.47608399391174</v>
+        <v>39.48555731773376</v>
       </c>
     </row>
     <row r="5">
@@ -573,7 +573,7 @@
         <v>104</v>
       </c>
       <c r="B5" t="n">
-        <v>2236</v>
+        <v>2232</v>
       </c>
       <c r="C5" t="n">
         <v>2228</v>
@@ -582,7 +582,7 @@
         <v>2225</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
         <v>2</v>
@@ -591,13 +591,13 @@
         <v>99.91019308486753</v>
       </c>
       <c r="H5" t="n">
-        <v>99.55257270693512</v>
+        <v>99.73106230389959</v>
       </c>
       <c r="I5" t="n">
-        <v>0.005385996409335727</v>
+        <v>0.003590664272890485</v>
       </c>
       <c r="J5" t="n">
-        <v>39.79212856292725</v>
+        <v>40.16272592544556</v>
       </c>
     </row>
     <row r="6">
@@ -605,31 +605,31 @@
         <v>105</v>
       </c>
       <c r="B6" t="n">
-        <v>2578</v>
+        <v>2576</v>
       </c>
       <c r="C6" t="n">
         <v>2571</v>
       </c>
       <c r="D6" t="n">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="E6" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G6" t="n">
-        <v>99.49416342412451</v>
+        <v>99.45525291828794</v>
       </c>
       <c r="H6" t="n">
-        <v>99.22390376406675</v>
+        <v>99.2621359223301</v>
       </c>
       <c r="I6" t="n">
         <v>0.01283547257876313</v>
       </c>
       <c r="J6" t="n">
-        <v>40.30218744277954</v>
+        <v>41.05736660957336</v>
       </c>
     </row>
     <row r="7">
@@ -661,7 +661,7 @@
         <v>0.001973359644795264</v>
       </c>
       <c r="J7" t="n">
-        <v>40.1474404335022</v>
+        <v>41.75398063659668</v>
       </c>
     </row>
     <row r="8">
@@ -669,7 +669,7 @@
         <v>107</v>
       </c>
       <c r="B8" t="n">
-        <v>2181</v>
+        <v>2139</v>
       </c>
       <c r="C8" t="n">
         <v>2135</v>
@@ -678,7 +678,7 @@
         <v>2133</v>
       </c>
       <c r="E8" t="n">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -687,13 +687,13 @@
         <v>99.95313964386129</v>
       </c>
       <c r="H8" t="n">
-        <v>97.8440366972477</v>
+        <v>99.76613657623948</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0224824355971897</v>
+        <v>0.002810304449648712</v>
       </c>
       <c r="J8" t="n">
-        <v>40.87517118453979</v>
+        <v>44.15846085548401</v>
       </c>
     </row>
     <row r="9">
@@ -701,7 +701,7 @@
         <v>108</v>
       </c>
       <c r="B9" t="n">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="C9" t="n">
         <v>1762</v>
@@ -710,7 +710,7 @@
         <v>1754</v>
       </c>
       <c r="E9" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" t="n">
         <v>7</v>
@@ -719,13 +719,13 @@
         <v>99.60249858035208</v>
       </c>
       <c r="H9" t="n">
-        <v>99.26428975664969</v>
+        <v>99.32049830124575</v>
       </c>
       <c r="I9" t="n">
-        <v>0.01135073779795687</v>
+        <v>0.01078320090805902</v>
       </c>
       <c r="J9" t="n">
-        <v>39.79865431785583</v>
+        <v>45.02007651329041</v>
       </c>
     </row>
     <row r="10">
@@ -757,7 +757,7 @@
         <v>0.002370604504148558</v>
       </c>
       <c r="J10" t="n">
-        <v>40.04406905174255</v>
+        <v>44.39277005195618</v>
       </c>
     </row>
     <row r="11">
@@ -789,7 +789,7 @@
         <v>0.001883239171374765</v>
       </c>
       <c r="J11" t="n">
-        <v>40.00422048568726</v>
+        <v>45.71279048919678</v>
       </c>
     </row>
     <row r="12">
@@ -797,7 +797,7 @@
         <v>112</v>
       </c>
       <c r="B12" t="n">
-        <v>2539</v>
+        <v>2538</v>
       </c>
       <c r="C12" t="n">
         <v>2538</v>
@@ -806,7 +806,7 @@
         <v>2537</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -815,13 +815,13 @@
         <v>100</v>
       </c>
       <c r="H12" t="n">
-        <v>99.96059889676911</v>
+        <v>100</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0003940110323089047</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>39.75757908821106</v>
+        <v>45.5863995552063</v>
       </c>
     </row>
     <row r="13">
@@ -829,7 +829,7 @@
         <v>113</v>
       </c>
       <c r="B13" t="n">
-        <v>1806</v>
+        <v>1795</v>
       </c>
       <c r="C13" t="n">
         <v>1795</v>
@@ -838,7 +838,7 @@
         <v>1793</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -847,13 +847,13 @@
         <v>99.94425863991081</v>
       </c>
       <c r="H13" t="n">
-        <v>99.33518005540166</v>
+        <v>99.94425863991081</v>
       </c>
       <c r="I13" t="n">
-        <v>0.007242339832869081</v>
+        <v>0.001114206128133705</v>
       </c>
       <c r="J13" t="n">
-        <v>39.88439130783081</v>
+        <v>46.052090883255</v>
       </c>
     </row>
     <row r="14">
@@ -861,7 +861,7 @@
         <v>114</v>
       </c>
       <c r="B14" t="n">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="C14" t="n">
         <v>1879</v>
@@ -870,7 +870,7 @@
         <v>1872</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
         <v>6</v>
@@ -879,13 +879,13 @@
         <v>99.68051118210863</v>
       </c>
       <c r="H14" t="n">
-        <v>99.68051118210863</v>
+        <v>99.73361747469366</v>
       </c>
       <c r="I14" t="n">
-        <v>0.006386375731772219</v>
+        <v>0.005854177754124534</v>
       </c>
       <c r="J14" t="n">
-        <v>39.70295524597168</v>
+        <v>44.654541015625</v>
       </c>
     </row>
     <row r="15">
@@ -917,7 +917,7 @@
         <v>0.0005120327700972862</v>
       </c>
       <c r="J15" t="n">
-        <v>39.24021124839783</v>
+        <v>42.44349765777588</v>
       </c>
     </row>
     <row r="16">
@@ -949,7 +949,7 @@
         <v>0.009954375777685608</v>
       </c>
       <c r="J16" t="n">
-        <v>40.54644918441772</v>
+        <v>44.30206179618835</v>
       </c>
     </row>
     <row r="17">
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>39.79909944534302</v>
+        <v>42.85961079597473</v>
       </c>
     </row>
     <row r="18">
@@ -989,7 +989,7 @@
         <v>118</v>
       </c>
       <c r="B18" t="n">
-        <v>2281</v>
+        <v>2279</v>
       </c>
       <c r="C18" t="n">
         <v>2276</v>
@@ -998,7 +998,7 @@
         <v>2275</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -1007,13 +1007,13 @@
         <v>100</v>
       </c>
       <c r="H18" t="n">
-        <v>99.78070175438596</v>
+        <v>99.86830553116769</v>
       </c>
       <c r="I18" t="n">
-        <v>0.002196836555360281</v>
+        <v>0.001318101933216169</v>
       </c>
       <c r="J18" t="n">
-        <v>40.52464532852173</v>
+        <v>43.35636258125305</v>
       </c>
     </row>
     <row r="19">
@@ -1021,7 +1021,7 @@
         <v>119</v>
       </c>
       <c r="B19" t="n">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="C19" t="n">
         <v>1987</v>
@@ -1030,7 +1030,7 @@
         <v>1986</v>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1039,13 +1039,13 @@
         <v>100</v>
       </c>
       <c r="H19" t="n">
-        <v>99.74886991461577</v>
+        <v>99.79899497487438</v>
       </c>
       <c r="I19" t="n">
-        <v>0.002516356316054353</v>
+        <v>0.002013085052843483</v>
       </c>
       <c r="J19" t="n">
-        <v>42.02813577651978</v>
+        <v>42.35549330711365</v>
       </c>
     </row>
     <row r="20">
@@ -1077,7 +1077,7 @@
         <v>0.001610305958132045</v>
       </c>
       <c r="J20" t="n">
-        <v>39.72353029251099</v>
+        <v>42.43965625762939</v>
       </c>
     </row>
     <row r="21">
@@ -1109,7 +1109,7 @@
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>40.10713529586792</v>
+        <v>43.16368007659912</v>
       </c>
     </row>
     <row r="22">
@@ -1117,7 +1117,7 @@
         <v>123</v>
       </c>
       <c r="B22" t="n">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="C22" t="n">
         <v>1517</v>
@@ -1126,7 +1126,7 @@
         <v>1516</v>
       </c>
       <c r="E22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1135,13 +1135,13 @@
         <v>100</v>
       </c>
       <c r="H22" t="n">
-        <v>99.86824769433466</v>
+        <v>99.9340804218853</v>
       </c>
       <c r="I22" t="n">
-        <v>0.001318391562294001</v>
+        <v>0.0006591957811470006</v>
       </c>
       <c r="J22" t="n">
-        <v>39.75511240959167</v>
+        <v>42.60353398323059</v>
       </c>
     </row>
     <row r="23">
@@ -1173,7 +1173,7 @@
         <v>0.001235330450895615</v>
       </c>
       <c r="J23" t="n">
-        <v>39.36995577812195</v>
+        <v>42.91984677314758</v>
       </c>
     </row>
     <row r="24">
@@ -1181,31 +1181,31 @@
         <v>200</v>
       </c>
       <c r="B24" t="n">
-        <v>2601</v>
+        <v>2600</v>
       </c>
       <c r="C24" t="n">
         <v>2601</v>
       </c>
       <c r="D24" t="n">
-        <v>2598</v>
+        <v>2597</v>
       </c>
       <c r="E24" t="n">
         <v>2</v>
       </c>
       <c r="F24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G24" t="n">
-        <v>99.92307692307692</v>
+        <v>99.88461538461539</v>
       </c>
       <c r="H24" t="n">
-        <v>99.92307692307692</v>
+        <v>99.92304732589457</v>
       </c>
       <c r="I24" t="n">
-        <v>0.001537870049980777</v>
+        <v>0.001922337562475971</v>
       </c>
       <c r="J24" t="n">
-        <v>40.043301820755</v>
+        <v>43.26388025283813</v>
       </c>
     </row>
     <row r="25">
@@ -1213,31 +1213,31 @@
         <v>201</v>
       </c>
       <c r="B25" t="n">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="C25" t="n">
         <v>1963</v>
       </c>
       <c r="D25" t="n">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G25" t="n">
-        <v>99.33741080530072</v>
+        <v>99.28644240570846</v>
       </c>
       <c r="H25" t="n">
-        <v>99.89748846745259</v>
+        <v>99.94869163673678</v>
       </c>
       <c r="I25" t="n">
         <v>0.007641365257259297</v>
       </c>
       <c r="J25" t="n">
-        <v>39.58996868133545</v>
+        <v>42.35196018218994</v>
       </c>
     </row>
     <row r="26">
@@ -1269,7 +1269,7 @@
         <v>0.005149812734082397</v>
       </c>
       <c r="J26" t="n">
-        <v>39.12427878379822</v>
+        <v>42.78260517120361</v>
       </c>
     </row>
     <row r="27">
@@ -1277,31 +1277,31 @@
         <v>203</v>
       </c>
       <c r="B27" t="n">
-        <v>2877</v>
+        <v>2765</v>
       </c>
       <c r="C27" t="n">
         <v>2979</v>
       </c>
       <c r="D27" t="n">
-        <v>2864</v>
+        <v>2752</v>
       </c>
       <c r="E27" t="n">
         <v>12</v>
       </c>
       <c r="F27" t="n">
-        <v>114</v>
+        <v>226</v>
       </c>
       <c r="G27" t="n">
-        <v>96.1719274680994</v>
+        <v>92.41101410342512</v>
       </c>
       <c r="H27" t="n">
-        <v>99.58275382475661</v>
+        <v>99.56584659913169</v>
       </c>
       <c r="I27" t="n">
-        <v>0.04229607250755287</v>
+        <v>0.07989258140315542</v>
       </c>
       <c r="J27" t="n">
-        <v>40.15285205841064</v>
+        <v>43.22052311897278</v>
       </c>
     </row>
     <row r="28">
@@ -1309,31 +1309,31 @@
         <v>205</v>
       </c>
       <c r="B28" t="n">
-        <v>2636</v>
+        <v>2634</v>
       </c>
       <c r="C28" t="n">
         <v>2656</v>
       </c>
       <c r="D28" t="n">
-        <v>2635</v>
+        <v>2633</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G28" t="n">
-        <v>99.24670433145009</v>
+        <v>99.1713747645951</v>
       </c>
       <c r="H28" t="n">
         <v>100</v>
       </c>
       <c r="I28" t="n">
-        <v>0.007530120481927711</v>
+        <v>0.008283132530120483</v>
       </c>
       <c r="J28" t="n">
-        <v>39.28722906112671</v>
+        <v>42.01884341239929</v>
       </c>
     </row>
     <row r="29">
@@ -1341,31 +1341,31 @@
         <v>207</v>
       </c>
       <c r="B29" t="n">
-        <v>2064</v>
+        <v>2048</v>
       </c>
       <c r="C29" t="n">
         <v>1859</v>
       </c>
       <c r="D29" t="n">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="E29" t="n">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="F29" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G29" t="n">
-        <v>99.67707212055974</v>
+        <v>99.62325080731969</v>
       </c>
       <c r="H29" t="n">
-        <v>89.77217644207465</v>
+        <v>90.42501221299463</v>
       </c>
       <c r="I29" t="n">
-        <v>0.1167294244217321</v>
+        <v>0.1091984938138784</v>
       </c>
       <c r="J29" t="n">
-        <v>39.38474154472351</v>
+        <v>42.05958461761475</v>
       </c>
     </row>
     <row r="30">
@@ -1373,7 +1373,7 @@
         <v>208</v>
       </c>
       <c r="B30" t="n">
-        <v>2944</v>
+        <v>2943</v>
       </c>
       <c r="C30" t="n">
         <v>2953</v>
@@ -1382,7 +1382,7 @@
         <v>2937</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="n">
         <v>15</v>
@@ -1391,13 +1391,13 @@
         <v>99.49186991869918</v>
       </c>
       <c r="H30" t="n">
-        <v>99.79612640163099</v>
+        <v>99.83004758667573</v>
       </c>
       <c r="I30" t="n">
-        <v>0.007111412123264477</v>
+        <v>0.006772773450728073</v>
       </c>
       <c r="J30" t="n">
-        <v>40.32072949409485</v>
+        <v>42.51695394515991</v>
       </c>
     </row>
     <row r="31">
@@ -1405,31 +1405,31 @@
         <v>209</v>
       </c>
       <c r="B31" t="n">
-        <v>3005</v>
+        <v>2996</v>
       </c>
       <c r="C31" t="n">
         <v>3005</v>
       </c>
       <c r="D31" t="n">
-        <v>3004</v>
+        <v>2995</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G31" t="n">
-        <v>100</v>
+        <v>99.70039946737683</v>
       </c>
       <c r="H31" t="n">
         <v>100</v>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>0.002995008319467554</v>
       </c>
       <c r="J31" t="n">
-        <v>40.25624775886536</v>
+        <v>42.76798915863037</v>
       </c>
     </row>
     <row r="32">
@@ -1437,31 +1437,31 @@
         <v>210</v>
       </c>
       <c r="B32" t="n">
-        <v>2624</v>
+        <v>2619</v>
       </c>
       <c r="C32" t="n">
         <v>2649</v>
       </c>
       <c r="D32" t="n">
-        <v>2621</v>
+        <v>2617</v>
       </c>
       <c r="E32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G32" t="n">
-        <v>98.98036253776435</v>
+        <v>98.82930513595166</v>
       </c>
       <c r="H32" t="n">
-        <v>99.9237514296607</v>
+        <v>99.96180290297937</v>
       </c>
       <c r="I32" t="n">
-        <v>0.01094752736881842</v>
+        <v>0.0120800302000755</v>
       </c>
       <c r="J32" t="n">
-        <v>39.3378758430481</v>
+        <v>42.06166124343872</v>
       </c>
     </row>
     <row r="33">
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>41.54549169540405</v>
+        <v>42.6504852771759</v>
       </c>
     </row>
     <row r="34">
@@ -1525,7 +1525,7 @@
         <v>0.001847290640394089</v>
       </c>
       <c r="J34" t="n">
-        <v>43.36691403388977</v>
+        <v>43.15852308273315</v>
       </c>
     </row>
     <row r="35">
@@ -1533,31 +1533,31 @@
         <v>214</v>
       </c>
       <c r="B35" t="n">
-        <v>2258</v>
+        <v>2256</v>
       </c>
       <c r="C35" t="n">
         <v>2261</v>
       </c>
       <c r="D35" t="n">
-        <v>2257</v>
+        <v>2255</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G35" t="n">
-        <v>99.86725663716814</v>
+        <v>99.77876106194691</v>
       </c>
       <c r="H35" t="n">
         <v>100</v>
       </c>
       <c r="I35" t="n">
-        <v>0.001326846528084918</v>
+        <v>0.00221141088014153</v>
       </c>
       <c r="J35" t="n">
-        <v>39.70415186882019</v>
+        <v>40.04944801330566</v>
       </c>
     </row>
     <row r="36">
@@ -1565,31 +1565,31 @@
         <v>215</v>
       </c>
       <c r="B36" t="n">
-        <v>3359</v>
+        <v>3343</v>
       </c>
       <c r="C36" t="n">
         <v>3362</v>
       </c>
       <c r="D36" t="n">
-        <v>3358</v>
+        <v>3342</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="G36" t="n">
-        <v>99.91074085093722</v>
+        <v>99.43469205593573</v>
       </c>
       <c r="H36" t="n">
         <v>100</v>
       </c>
       <c r="I36" t="n">
-        <v>0.000892325996430696</v>
+        <v>0.005651397977394408</v>
       </c>
       <c r="J36" t="n">
-        <v>40.79715967178345</v>
+        <v>40.97624850273132</v>
       </c>
     </row>
     <row r="37">
@@ -1597,7 +1597,7 @@
         <v>217</v>
       </c>
       <c r="B37" t="n">
-        <v>3282</v>
+        <v>2295</v>
       </c>
       <c r="C37" t="n">
         <v>2208</v>
@@ -1606,7 +1606,7 @@
         <v>2203</v>
       </c>
       <c r="E37" t="n">
-        <v>1078</v>
+        <v>91</v>
       </c>
       <c r="F37" t="n">
         <v>4</v>
@@ -1615,13 +1615,13 @@
         <v>99.81875849569552</v>
       </c>
       <c r="H37" t="n">
-        <v>67.14416336482779</v>
+        <v>96.03312990409765</v>
       </c>
       <c r="I37" t="n">
-        <v>0.490036231884058</v>
+        <v>0.04302536231884058</v>
       </c>
       <c r="J37" t="n">
-        <v>40.4207935333252</v>
+        <v>41.48243403434753</v>
       </c>
     </row>
     <row r="38">
@@ -1653,7 +1653,7 @@
         <v>0.0004642525533890436</v>
       </c>
       <c r="J38" t="n">
-        <v>39.61178946495056</v>
+        <v>40.40843796730042</v>
       </c>
     </row>
     <row r="39">
@@ -1685,7 +1685,7 @@
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>40.35430788993835</v>
+        <v>40.19192481040955</v>
       </c>
     </row>
     <row r="40">
@@ -1717,7 +1717,7 @@
         <v>0.002472187886279357</v>
       </c>
       <c r="J40" t="n">
-        <v>39.30700588226318</v>
+        <v>39.76478838920593</v>
       </c>
     </row>
     <row r="41">
@@ -1725,31 +1725,31 @@
         <v>222</v>
       </c>
       <c r="B41" t="n">
-        <v>2485</v>
+        <v>2480</v>
       </c>
       <c r="C41" t="n">
         <v>2482</v>
       </c>
       <c r="D41" t="n">
-        <v>2479</v>
+        <v>2474</v>
       </c>
       <c r="E41" t="n">
         <v>5</v>
       </c>
       <c r="F41" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G41" t="n">
-        <v>99.91938734381299</v>
+        <v>99.71785570334542</v>
       </c>
       <c r="H41" t="n">
-        <v>99.7987117552335</v>
+        <v>99.79830576845502</v>
       </c>
       <c r="I41" t="n">
-        <v>0.00282030620467365</v>
+        <v>0.004834810636583401</v>
       </c>
       <c r="J41" t="n">
-        <v>39.79197692871094</v>
+        <v>40.27411818504333</v>
       </c>
     </row>
     <row r="42">
@@ -1781,7 +1781,7 @@
         <v>0.004990403071017275</v>
       </c>
       <c r="J42" t="n">
-        <v>40.09335041046143</v>
+        <v>39.99424004554749</v>
       </c>
     </row>
     <row r="43">
@@ -1789,7 +1789,7 @@
         <v>228</v>
       </c>
       <c r="B43" t="n">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="C43" t="n">
         <v>2052</v>
@@ -1798,7 +1798,7 @@
         <v>2044</v>
       </c>
       <c r="E43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F43" t="n">
         <v>7</v>
@@ -1807,13 +1807,13 @@
         <v>99.65870307167235</v>
       </c>
       <c r="H43" t="n">
-        <v>99.65870307167235</v>
+        <v>99.70731707317073</v>
       </c>
       <c r="I43" t="n">
-        <v>0.00682261208576998</v>
+        <v>0.006335282651072124</v>
       </c>
       <c r="J43" t="n">
-        <v>39.88975071907043</v>
+        <v>40.10549712181091</v>
       </c>
     </row>
     <row r="44">
@@ -1821,7 +1821,7 @@
         <v>230</v>
       </c>
       <c r="B44" t="n">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="C44" t="n">
         <v>2255</v>
@@ -1830,7 +1830,7 @@
         <v>2254</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
@@ -1839,13 +1839,13 @@
         <v>100</v>
       </c>
       <c r="H44" t="n">
-        <v>99.95565410199556</v>
+        <v>100</v>
       </c>
       <c r="I44" t="n">
-        <v>0.0004434589800443459</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>40.35441946983337</v>
+        <v>40.19294333457947</v>
       </c>
     </row>
     <row r="45">
@@ -1853,7 +1853,7 @@
         <v>231</v>
       </c>
       <c r="B45" t="n">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="C45" t="n">
         <v>1570</v>
@@ -1862,7 +1862,7 @@
         <v>1569</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -1871,13 +1871,13 @@
         <v>100</v>
       </c>
       <c r="H45" t="n">
-        <v>99.87269255251432</v>
+        <v>99.93630573248407</v>
       </c>
       <c r="I45" t="n">
-        <v>0.001273885350318471</v>
+        <v>0.0006369426751592356</v>
       </c>
       <c r="J45" t="n">
-        <v>39.83396649360657</v>
+        <v>39.69635796546936</v>
       </c>
     </row>
     <row r="46">
@@ -1885,7 +1885,7 @@
         <v>232</v>
       </c>
       <c r="B46" t="n">
-        <v>1785</v>
+        <v>1783</v>
       </c>
       <c r="C46" t="n">
         <v>1780</v>
@@ -1894,7 +1894,7 @@
         <v>1779</v>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -1903,13 +1903,13 @@
         <v>100</v>
       </c>
       <c r="H46" t="n">
-        <v>99.71973094170404</v>
+        <v>99.83164983164983</v>
       </c>
       <c r="I46" t="n">
-        <v>0.002808988764044944</v>
+        <v>0.001685393258426966</v>
       </c>
       <c r="J46" t="n">
-        <v>39.27898764610291</v>
+        <v>39.73055195808411</v>
       </c>
     </row>
     <row r="47">
@@ -1917,31 +1917,31 @@
         <v>233</v>
       </c>
       <c r="B47" t="n">
-        <v>3078</v>
+        <v>3055</v>
       </c>
       <c r="C47" t="n">
         <v>3077</v>
       </c>
       <c r="D47" t="n">
-        <v>3076</v>
+        <v>3053</v>
       </c>
       <c r="E47" t="n">
         <v>1</v>
       </c>
       <c r="F47" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G47" t="n">
-        <v>100</v>
+        <v>99.25227568270481</v>
       </c>
       <c r="H47" t="n">
-        <v>99.96750081247968</v>
+        <v>99.96725605762934</v>
       </c>
       <c r="I47" t="n">
-        <v>0.0003249918752031199</v>
+        <v>0.007799805004874878</v>
       </c>
       <c r="J47" t="n">
-        <v>41.00643682479858</v>
+        <v>41.0127592086792</v>
       </c>
     </row>
     <row r="48">
@@ -1973,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>40.17040872573853</v>
+        <v>40.36393451690674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
including afib annotation and searching a peak in 2*b interva;
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/attempt1.xlsx
+++ b/R peak detection/beatdetection/attempt1.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="sdfewf" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="nadibf" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>39.11275243759155</v>
+        <v>42.04670763015747</v>
       </c>
     </row>
     <row r="2">
@@ -501,7 +501,7 @@
         <v>0.000536480686695279</v>
       </c>
       <c r="J2" t="n">
-        <v>38.96059703826904</v>
+        <v>40.82866406440735</v>
       </c>
     </row>
     <row r="3">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>39.64492177963257</v>
+        <v>40.51431345939636</v>
       </c>
     </row>
     <row r="4">
@@ -565,7 +565,7 @@
         <v>0.0004798464491362764</v>
       </c>
       <c r="J4" t="n">
-        <v>39.48555731773376</v>
+        <v>42.34519624710083</v>
       </c>
     </row>
     <row r="5">
@@ -573,31 +573,31 @@
         <v>104</v>
       </c>
       <c r="B5" t="n">
-        <v>2232</v>
+        <v>2235</v>
       </c>
       <c r="C5" t="n">
         <v>2228</v>
       </c>
       <c r="D5" t="n">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" t="n">
-        <v>99.91019308486753</v>
+        <v>99.86528962730131</v>
       </c>
       <c r="H5" t="n">
-        <v>99.73106230389959</v>
+        <v>99.55237242614145</v>
       </c>
       <c r="I5" t="n">
-        <v>0.003590664272890485</v>
+        <v>0.005834829443447037</v>
       </c>
       <c r="J5" t="n">
-        <v>40.16272592544556</v>
+        <v>41.70451474189758</v>
       </c>
     </row>
     <row r="6">
@@ -605,7 +605,7 @@
         <v>105</v>
       </c>
       <c r="B6" t="n">
-        <v>2576</v>
+        <v>2584</v>
       </c>
       <c r="C6" t="n">
         <v>2571</v>
@@ -614,7 +614,7 @@
         <v>2556</v>
       </c>
       <c r="E6" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F6" t="n">
         <v>14</v>
@@ -623,13 +623,13 @@
         <v>99.45525291828794</v>
       </c>
       <c r="H6" t="n">
-        <v>99.2621359223301</v>
+        <v>98.95470383275261</v>
       </c>
       <c r="I6" t="n">
-        <v>0.01283547257876313</v>
+        <v>0.01594710229482691</v>
       </c>
       <c r="J6" t="n">
-        <v>41.05736660957336</v>
+        <v>41.18650507926941</v>
       </c>
     </row>
     <row r="7">
@@ -637,7 +637,7 @@
         <v>106</v>
       </c>
       <c r="B7" t="n">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="C7" t="n">
         <v>2027</v>
@@ -646,7 +646,7 @@
         <v>2023</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>3</v>
@@ -655,13 +655,13 @@
         <v>99.85192497532083</v>
       </c>
       <c r="H7" t="n">
-        <v>99.9505928853755</v>
+        <v>99.90123456790124</v>
       </c>
       <c r="I7" t="n">
-        <v>0.001973359644795264</v>
+        <v>0.00246669955599408</v>
       </c>
       <c r="J7" t="n">
-        <v>41.75398063659668</v>
+        <v>43.21181845664978</v>
       </c>
     </row>
     <row r="8">
@@ -669,7 +669,7 @@
         <v>107</v>
       </c>
       <c r="B8" t="n">
-        <v>2139</v>
+        <v>2222</v>
       </c>
       <c r="C8" t="n">
         <v>2135</v>
@@ -678,7 +678,7 @@
         <v>2133</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="F8" t="n">
         <v>1</v>
@@ -687,13 +687,13 @@
         <v>99.95313964386129</v>
       </c>
       <c r="H8" t="n">
-        <v>99.76613657623948</v>
+        <v>96.03782080144079</v>
       </c>
       <c r="I8" t="n">
-        <v>0.002810304449648712</v>
+        <v>0.04168618266978923</v>
       </c>
       <c r="J8" t="n">
-        <v>44.15846085548401</v>
+        <v>42.3247447013855</v>
       </c>
     </row>
     <row r="9">
@@ -701,7 +701,7 @@
         <v>108</v>
       </c>
       <c r="B9" t="n">
-        <v>1767</v>
+        <v>1768</v>
       </c>
       <c r="C9" t="n">
         <v>1762</v>
@@ -710,7 +710,7 @@
         <v>1754</v>
       </c>
       <c r="E9" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F9" t="n">
         <v>7</v>
@@ -719,13 +719,13 @@
         <v>99.60249858035208</v>
       </c>
       <c r="H9" t="n">
-        <v>99.32049830124575</v>
+        <v>99.26428975664969</v>
       </c>
       <c r="I9" t="n">
-        <v>0.01078320090805902</v>
+        <v>0.01135073779795687</v>
       </c>
       <c r="J9" t="n">
-        <v>45.02007651329041</v>
+        <v>39.94191884994507</v>
       </c>
     </row>
     <row r="10">
@@ -757,7 +757,7 @@
         <v>0.002370604504148558</v>
       </c>
       <c r="J10" t="n">
-        <v>44.39277005195618</v>
+        <v>39.85851001739502</v>
       </c>
     </row>
     <row r="11">
@@ -789,7 +789,7 @@
         <v>0.001883239171374765</v>
       </c>
       <c r="J11" t="n">
-        <v>45.71279048919678</v>
+        <v>40.13940715789795</v>
       </c>
     </row>
     <row r="12">
@@ -797,7 +797,7 @@
         <v>112</v>
       </c>
       <c r="B12" t="n">
-        <v>2538</v>
+        <v>2559</v>
       </c>
       <c r="C12" t="n">
         <v>2538</v>
@@ -806,7 +806,7 @@
         <v>2537</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -815,13 +815,13 @@
         <v>100</v>
       </c>
       <c r="H12" t="n">
-        <v>100</v>
+        <v>99.1790461297889</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>0.008274231678486997</v>
       </c>
       <c r="J12" t="n">
-        <v>45.5863995552063</v>
+        <v>39.72089266777039</v>
       </c>
     </row>
     <row r="13">
@@ -829,7 +829,7 @@
         <v>113</v>
       </c>
       <c r="B13" t="n">
-        <v>1795</v>
+        <v>1812</v>
       </c>
       <c r="C13" t="n">
         <v>1795</v>
@@ -838,7 +838,7 @@
         <v>1793</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -847,13 +847,13 @@
         <v>99.94425863991081</v>
       </c>
       <c r="H13" t="n">
-        <v>99.94425863991081</v>
+        <v>99.00607399226946</v>
       </c>
       <c r="I13" t="n">
-        <v>0.001114206128133705</v>
+        <v>0.0105849582172702</v>
       </c>
       <c r="J13" t="n">
-        <v>46.052090883255</v>
+        <v>39.43358469009399</v>
       </c>
     </row>
     <row r="14">
@@ -885,7 +885,7 @@
         <v>0.005854177754124534</v>
       </c>
       <c r="J14" t="n">
-        <v>44.654541015625</v>
+        <v>39.27301263809204</v>
       </c>
     </row>
     <row r="15">
@@ -917,7 +917,7 @@
         <v>0.0005120327700972862</v>
       </c>
       <c r="J15" t="n">
-        <v>42.44349765777588</v>
+        <v>38.85359668731689</v>
       </c>
     </row>
     <row r="16">
@@ -949,7 +949,7 @@
         <v>0.009954375777685608</v>
       </c>
       <c r="J16" t="n">
-        <v>44.30206179618835</v>
+        <v>40.73881936073303</v>
       </c>
     </row>
     <row r="17">
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>42.85961079597473</v>
+        <v>39.66579484939575</v>
       </c>
     </row>
     <row r="18">
@@ -1013,7 +1013,7 @@
         <v>0.001318101933216169</v>
       </c>
       <c r="J18" t="n">
-        <v>43.35636258125305</v>
+        <v>41.65223956108093</v>
       </c>
     </row>
     <row r="19">
@@ -1021,7 +1021,7 @@
         <v>119</v>
       </c>
       <c r="B19" t="n">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="C19" t="n">
         <v>1987</v>
@@ -1030,7 +1030,7 @@
         <v>1986</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1039,13 +1039,13 @@
         <v>100</v>
       </c>
       <c r="H19" t="n">
-        <v>99.79899497487438</v>
+        <v>99.74886991461577</v>
       </c>
       <c r="I19" t="n">
-        <v>0.002013085052843483</v>
+        <v>0.002516356316054353</v>
       </c>
       <c r="J19" t="n">
-        <v>42.35549330711365</v>
+        <v>40.30982542037964</v>
       </c>
     </row>
     <row r="20">
@@ -1077,7 +1077,7 @@
         <v>0.001610305958132045</v>
       </c>
       <c r="J20" t="n">
-        <v>42.43965625762939</v>
+        <v>39.63760089874268</v>
       </c>
     </row>
     <row r="21">
@@ -1109,7 +1109,7 @@
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>43.16368007659912</v>
+        <v>40.67124652862549</v>
       </c>
     </row>
     <row r="22">
@@ -1117,7 +1117,7 @@
         <v>123</v>
       </c>
       <c r="B22" t="n">
-        <v>1518</v>
+        <v>1520</v>
       </c>
       <c r="C22" t="n">
         <v>1517</v>
@@ -1126,7 +1126,7 @@
         <v>1516</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1135,13 +1135,13 @@
         <v>100</v>
       </c>
       <c r="H22" t="n">
-        <v>99.9340804218853</v>
+        <v>99.80250164581962</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0006591957811470006</v>
+        <v>0.001977587343441002</v>
       </c>
       <c r="J22" t="n">
-        <v>42.60353398323059</v>
+        <v>39.27433133125305</v>
       </c>
     </row>
     <row r="23">
@@ -1173,7 +1173,7 @@
         <v>0.001235330450895615</v>
       </c>
       <c r="J23" t="n">
-        <v>42.91984677314758</v>
+        <v>39.93972229957581</v>
       </c>
     </row>
     <row r="24">
@@ -1181,31 +1181,31 @@
         <v>200</v>
       </c>
       <c r="B24" t="n">
-        <v>2600</v>
+        <v>2601</v>
       </c>
       <c r="C24" t="n">
         <v>2601</v>
       </c>
       <c r="D24" t="n">
-        <v>2597</v>
+        <v>2598</v>
       </c>
       <c r="E24" t="n">
         <v>2</v>
       </c>
       <c r="F24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G24" t="n">
-        <v>99.88461538461539</v>
+        <v>99.92307692307692</v>
       </c>
       <c r="H24" t="n">
-        <v>99.92304732589457</v>
+        <v>99.92307692307692</v>
       </c>
       <c r="I24" t="n">
-        <v>0.001922337562475971</v>
+        <v>0.001537870049980777</v>
       </c>
       <c r="J24" t="n">
-        <v>43.26388025283813</v>
+        <v>40.18035435676575</v>
       </c>
     </row>
     <row r="25">
@@ -1213,31 +1213,31 @@
         <v>201</v>
       </c>
       <c r="B25" t="n">
-        <v>1950</v>
+        <v>1951</v>
       </c>
       <c r="C25" t="n">
         <v>1963</v>
       </c>
       <c r="D25" t="n">
-        <v>1948</v>
+        <v>1949</v>
       </c>
       <c r="E25" t="n">
         <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G25" t="n">
-        <v>99.28644240570846</v>
+        <v>99.33741080530072</v>
       </c>
       <c r="H25" t="n">
-        <v>99.94869163673678</v>
+        <v>99.94871794871794</v>
       </c>
       <c r="I25" t="n">
-        <v>0.007641365257259297</v>
+        <v>0.007131940906775344</v>
       </c>
       <c r="J25" t="n">
-        <v>42.35196018218994</v>
+        <v>39.88451290130615</v>
       </c>
     </row>
     <row r="26">
@@ -1269,7 +1269,7 @@
         <v>0.005149812734082397</v>
       </c>
       <c r="J26" t="n">
-        <v>42.78260517120361</v>
+        <v>41.18431997299194</v>
       </c>
     </row>
     <row r="27">
@@ -1277,31 +1277,31 @@
         <v>203</v>
       </c>
       <c r="B27" t="n">
-        <v>2765</v>
+        <v>2883</v>
       </c>
       <c r="C27" t="n">
         <v>2979</v>
       </c>
       <c r="D27" t="n">
-        <v>2752</v>
+        <v>2868</v>
       </c>
       <c r="E27" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F27" t="n">
-        <v>226</v>
+        <v>110</v>
       </c>
       <c r="G27" t="n">
-        <v>92.41101410342512</v>
+        <v>96.30624580255204</v>
       </c>
       <c r="H27" t="n">
-        <v>99.56584659913169</v>
+        <v>99.51422623178348</v>
       </c>
       <c r="I27" t="n">
-        <v>0.07989258140315542</v>
+        <v>0.04162470627727426</v>
       </c>
       <c r="J27" t="n">
-        <v>43.22052311897278</v>
+        <v>40.62373661994934</v>
       </c>
     </row>
     <row r="28">
@@ -1309,31 +1309,31 @@
         <v>205</v>
       </c>
       <c r="B28" t="n">
-        <v>2634</v>
+        <v>2636</v>
       </c>
       <c r="C28" t="n">
         <v>2656</v>
       </c>
       <c r="D28" t="n">
-        <v>2633</v>
+        <v>2635</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G28" t="n">
-        <v>99.1713747645951</v>
+        <v>99.24670433145009</v>
       </c>
       <c r="H28" t="n">
         <v>100</v>
       </c>
       <c r="I28" t="n">
-        <v>0.008283132530120483</v>
+        <v>0.007530120481927711</v>
       </c>
       <c r="J28" t="n">
-        <v>42.01884341239929</v>
+        <v>39.78992247581482</v>
       </c>
     </row>
     <row r="29">
@@ -1341,31 +1341,31 @@
         <v>207</v>
       </c>
       <c r="B29" t="n">
-        <v>2048</v>
+        <v>2086</v>
       </c>
       <c r="C29" t="n">
-        <v>1859</v>
+        <v>2331</v>
       </c>
       <c r="D29" t="n">
-        <v>1851</v>
+        <v>2075</v>
       </c>
       <c r="E29" t="n">
-        <v>196</v>
+        <v>10</v>
       </c>
       <c r="F29" t="n">
-        <v>7</v>
+        <v>255</v>
       </c>
       <c r="G29" t="n">
-        <v>99.62325080731969</v>
+        <v>89.05579399141631</v>
       </c>
       <c r="H29" t="n">
-        <v>90.42501221299463</v>
+        <v>99.52038369304556</v>
       </c>
       <c r="I29" t="n">
-        <v>0.1091984938138784</v>
+        <v>0.1136851136851137</v>
       </c>
       <c r="J29" t="n">
-        <v>42.05958461761475</v>
+        <v>39.48236966133118</v>
       </c>
     </row>
     <row r="30">
@@ -1373,31 +1373,31 @@
         <v>208</v>
       </c>
       <c r="B30" t="n">
-        <v>2943</v>
+        <v>2945</v>
       </c>
       <c r="C30" t="n">
         <v>2953</v>
       </c>
       <c r="D30" t="n">
-        <v>2937</v>
+        <v>2936</v>
       </c>
       <c r="E30" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F30" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G30" t="n">
-        <v>99.49186991869918</v>
+        <v>99.4579945799458</v>
       </c>
       <c r="H30" t="n">
-        <v>99.83004758667573</v>
+        <v>99.72826086956522</v>
       </c>
       <c r="I30" t="n">
-        <v>0.006772773450728073</v>
+        <v>0.008127328140873687</v>
       </c>
       <c r="J30" t="n">
-        <v>42.51695394515991</v>
+        <v>40.15036797523499</v>
       </c>
     </row>
     <row r="31">
@@ -1405,31 +1405,31 @@
         <v>209</v>
       </c>
       <c r="B31" t="n">
-        <v>2996</v>
+        <v>3005</v>
       </c>
       <c r="C31" t="n">
         <v>3005</v>
       </c>
       <c r="D31" t="n">
-        <v>2995</v>
+        <v>3004</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>99.70039946737683</v>
+        <v>100</v>
       </c>
       <c r="H31" t="n">
         <v>100</v>
       </c>
       <c r="I31" t="n">
-        <v>0.002995008319467554</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>42.76798915863037</v>
+        <v>40.37878513336182</v>
       </c>
     </row>
     <row r="32">
@@ -1437,31 +1437,31 @@
         <v>210</v>
       </c>
       <c r="B32" t="n">
-        <v>2619</v>
+        <v>2625</v>
       </c>
       <c r="C32" t="n">
         <v>2649</v>
       </c>
       <c r="D32" t="n">
-        <v>2617</v>
+        <v>2622</v>
       </c>
       <c r="E32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F32" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G32" t="n">
-        <v>98.82930513595166</v>
+        <v>99.01812688821752</v>
       </c>
       <c r="H32" t="n">
-        <v>99.96180290297937</v>
+        <v>99.92378048780488</v>
       </c>
       <c r="I32" t="n">
-        <v>0.0120800302000755</v>
+        <v>0.01057002642506606</v>
       </c>
       <c r="J32" t="n">
-        <v>42.06166124343872</v>
+        <v>39.32681894302368</v>
       </c>
     </row>
     <row r="33">
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>42.6504852771759</v>
+        <v>44.94929528236389</v>
       </c>
     </row>
     <row r="34">
@@ -1525,7 +1525,7 @@
         <v>0.001847290640394089</v>
       </c>
       <c r="J34" t="n">
-        <v>43.15852308273315</v>
+        <v>45.38955593109131</v>
       </c>
     </row>
     <row r="35">
@@ -1533,31 +1533,31 @@
         <v>214</v>
       </c>
       <c r="B35" t="n">
-        <v>2256</v>
+        <v>2257</v>
       </c>
       <c r="C35" t="n">
         <v>2261</v>
       </c>
       <c r="D35" t="n">
-        <v>2255</v>
+        <v>2256</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G35" t="n">
-        <v>99.77876106194691</v>
+        <v>99.82300884955752</v>
       </c>
       <c r="H35" t="n">
         <v>100</v>
       </c>
       <c r="I35" t="n">
-        <v>0.00221141088014153</v>
+        <v>0.001769128704113224</v>
       </c>
       <c r="J35" t="n">
-        <v>40.04944801330566</v>
+        <v>42.1408371925354</v>
       </c>
     </row>
     <row r="36">
@@ -1565,31 +1565,31 @@
         <v>215</v>
       </c>
       <c r="B36" t="n">
-        <v>3343</v>
+        <v>3358</v>
       </c>
       <c r="C36" t="n">
         <v>3362</v>
       </c>
       <c r="D36" t="n">
-        <v>3342</v>
+        <v>3357</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="G36" t="n">
-        <v>99.43469205593573</v>
+        <v>99.88098780124963</v>
       </c>
       <c r="H36" t="n">
         <v>100</v>
       </c>
       <c r="I36" t="n">
-        <v>0.005651397977394408</v>
+        <v>0.001189767995240928</v>
       </c>
       <c r="J36" t="n">
-        <v>40.97624850273132</v>
+        <v>43.1296055316925</v>
       </c>
     </row>
     <row r="37">
@@ -1597,7 +1597,7 @@
         <v>217</v>
       </c>
       <c r="B37" t="n">
-        <v>2295</v>
+        <v>2253</v>
       </c>
       <c r="C37" t="n">
         <v>2208</v>
@@ -1606,7 +1606,7 @@
         <v>2203</v>
       </c>
       <c r="E37" t="n">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="F37" t="n">
         <v>4</v>
@@ -1615,13 +1615,13 @@
         <v>99.81875849569552</v>
       </c>
       <c r="H37" t="n">
-        <v>96.03312990409765</v>
+        <v>97.82415630550622</v>
       </c>
       <c r="I37" t="n">
-        <v>0.04302536231884058</v>
+        <v>0.0240036231884058</v>
       </c>
       <c r="J37" t="n">
-        <v>41.48243403434753</v>
+        <v>42.35402250289917</v>
       </c>
     </row>
     <row r="38">
@@ -1653,7 +1653,7 @@
         <v>0.0004642525533890436</v>
       </c>
       <c r="J38" t="n">
-        <v>40.40843796730042</v>
+        <v>40.29392242431641</v>
       </c>
     </row>
     <row r="39">
@@ -1685,7 +1685,7 @@
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>40.19192481040955</v>
+        <v>40.13136625289917</v>
       </c>
     </row>
     <row r="40">
@@ -1717,7 +1717,7 @@
         <v>0.002472187886279357</v>
       </c>
       <c r="J40" t="n">
-        <v>39.76478838920593</v>
+        <v>40.02736830711365</v>
       </c>
     </row>
     <row r="41">
@@ -1725,31 +1725,31 @@
         <v>222</v>
       </c>
       <c r="B41" t="n">
-        <v>2480</v>
+        <v>2486</v>
       </c>
       <c r="C41" t="n">
         <v>2482</v>
       </c>
       <c r="D41" t="n">
-        <v>2474</v>
+        <v>2480</v>
       </c>
       <c r="E41" t="n">
         <v>5</v>
       </c>
       <c r="F41" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G41" t="n">
-        <v>99.71785570334542</v>
+        <v>99.95969367190649</v>
       </c>
       <c r="H41" t="n">
-        <v>99.79830576845502</v>
+        <v>99.79879275653923</v>
       </c>
       <c r="I41" t="n">
-        <v>0.004834810636583401</v>
+        <v>0.0024174053182917</v>
       </c>
       <c r="J41" t="n">
-        <v>40.27411818504333</v>
+        <v>40.13996267318726</v>
       </c>
     </row>
     <row r="42">
@@ -1781,7 +1781,7 @@
         <v>0.004990403071017275</v>
       </c>
       <c r="J42" t="n">
-        <v>39.99424004554749</v>
+        <v>40.51850080490112</v>
       </c>
     </row>
     <row r="43">
@@ -1789,7 +1789,7 @@
         <v>228</v>
       </c>
       <c r="B43" t="n">
-        <v>2051</v>
+        <v>2054</v>
       </c>
       <c r="C43" t="n">
         <v>2052</v>
@@ -1798,7 +1798,7 @@
         <v>2044</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F43" t="n">
         <v>7</v>
@@ -1807,13 +1807,13 @@
         <v>99.65870307167235</v>
       </c>
       <c r="H43" t="n">
-        <v>99.70731707317073</v>
+        <v>99.56161714564053</v>
       </c>
       <c r="I43" t="n">
-        <v>0.006335282651072124</v>
+        <v>0.007797270955165692</v>
       </c>
       <c r="J43" t="n">
-        <v>40.10549712181091</v>
+        <v>40.27977967262268</v>
       </c>
     </row>
     <row r="44">
@@ -1821,7 +1821,7 @@
         <v>230</v>
       </c>
       <c r="B44" t="n">
-        <v>2255</v>
+        <v>2256</v>
       </c>
       <c r="C44" t="n">
         <v>2255</v>
@@ -1830,7 +1830,7 @@
         <v>2254</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
@@ -1839,13 +1839,13 @@
         <v>100</v>
       </c>
       <c r="H44" t="n">
-        <v>100</v>
+        <v>99.95565410199556</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>0.0004434589800443459</v>
       </c>
       <c r="J44" t="n">
-        <v>40.19294333457947</v>
+        <v>40.15129661560059</v>
       </c>
     </row>
     <row r="45">
@@ -1853,7 +1853,7 @@
         <v>231</v>
       </c>
       <c r="B45" t="n">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="C45" t="n">
         <v>1570</v>
@@ -1862,7 +1862,7 @@
         <v>1569</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -1871,13 +1871,13 @@
         <v>100</v>
       </c>
       <c r="H45" t="n">
-        <v>99.93630573248407</v>
+        <v>99.87269255251432</v>
       </c>
       <c r="I45" t="n">
-        <v>0.0006369426751592356</v>
+        <v>0.001273885350318471</v>
       </c>
       <c r="J45" t="n">
-        <v>39.69635796546936</v>
+        <v>39.85698246955872</v>
       </c>
     </row>
     <row r="46">
@@ -1885,7 +1885,7 @@
         <v>232</v>
       </c>
       <c r="B46" t="n">
-        <v>1783</v>
+        <v>1786</v>
       </c>
       <c r="C46" t="n">
         <v>1780</v>
@@ -1894,7 +1894,7 @@
         <v>1779</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -1903,13 +1903,13 @@
         <v>100</v>
       </c>
       <c r="H46" t="n">
-        <v>99.83164983164983</v>
+        <v>99.66386554621849</v>
       </c>
       <c r="I46" t="n">
-        <v>0.001685393258426966</v>
+        <v>0.003370786516853933</v>
       </c>
       <c r="J46" t="n">
-        <v>39.73055195808411</v>
+        <v>40.05977582931519</v>
       </c>
     </row>
     <row r="47">
@@ -1917,31 +1917,31 @@
         <v>233</v>
       </c>
       <c r="B47" t="n">
-        <v>3055</v>
+        <v>3076</v>
       </c>
       <c r="C47" t="n">
         <v>3077</v>
       </c>
       <c r="D47" t="n">
-        <v>3053</v>
+        <v>3074</v>
       </c>
       <c r="E47" t="n">
         <v>1</v>
       </c>
       <c r="F47" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="G47" t="n">
-        <v>99.25227568270481</v>
+        <v>99.93498049414825</v>
       </c>
       <c r="H47" t="n">
-        <v>99.96725605762934</v>
+        <v>99.96747967479675</v>
       </c>
       <c r="I47" t="n">
-        <v>0.007799805004874878</v>
+        <v>0.0009749756256093598</v>
       </c>
       <c r="J47" t="n">
-        <v>41.0127592086792</v>
+        <v>42.01871585845947</v>
       </c>
     </row>
     <row r="48">
@@ -1973,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>40.36393451690674</v>
+        <v>41.22881722450256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating r peak detection
</commit_message>
<xml_diff>
--- a/R peak detection/beatdetection/attempt1.xlsx
+++ b/R peak detection/beatdetection/attempt1.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="jxid" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,19 +442,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="B1" t="n">
-        <v>1630</v>
+        <v>2272</v>
       </c>
       <c r="C1" t="n">
-        <v>1622</v>
+        <v>2272</v>
       </c>
       <c r="D1" t="n">
-        <v>1621</v>
+        <v>2271</v>
       </c>
       <c r="E1" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F1" t="n">
         <v>0</v>
@@ -463,62 +463,62 @@
         <v>100</v>
       </c>
       <c r="H1" t="n">
-        <v>99.50890116635973</v>
+        <v>100</v>
       </c>
       <c r="I1" t="n">
-        <v>0.004932182490752158</v>
+        <v>0</v>
       </c>
       <c r="J1" t="n">
-        <v>60.24558568000793</v>
+        <v>38.89905500411987</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>101</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1865</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1864</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1862</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
-        <v>2595</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2595</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2594</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>99.94632313472893</v>
       </c>
       <c r="H2" t="n">
-        <v>100</v>
+        <v>99.89270386266094</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>0.001609442060085837</v>
       </c>
       <c r="J2" t="n">
-        <v>62.39537477493286</v>
+        <v>39.14367651939392</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="B3" t="n">
-        <v>2197</v>
+        <v>2186</v>
       </c>
       <c r="C3" t="n">
-        <v>2181</v>
+        <v>2186</v>
       </c>
       <c r="D3" t="n">
-        <v>2180</v>
+        <v>2185</v>
       </c>
       <c r="E3" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -527,45 +527,1453 @@
         <v>100</v>
       </c>
       <c r="H3" t="n">
-        <v>99.27140255009107</v>
+        <v>100</v>
       </c>
       <c r="I3" t="n">
-        <v>0.007336084364970197</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>61.04466962814331</v>
+        <v>38.99779629707336</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
+        <v>103</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2083</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2084</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2082</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>99.951992318771</v>
+      </c>
+      <c r="H4" t="n">
+        <v>100</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.0004798464491362764</v>
+      </c>
+      <c r="J4" t="n">
+        <v>39.44967031478882</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>104</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2229</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2228</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2222</v>
+      </c>
+      <c r="E5" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" t="n">
+        <v>99.77548271216884</v>
+      </c>
+      <c r="H5" t="n">
+        <v>99.73070017953322</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.004937163375224416</v>
+      </c>
+      <c r="J5" t="n">
+        <v>39.3215799331665</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>105</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2574</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2571</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2551</v>
+      </c>
+      <c r="E6" t="n">
+        <v>22</v>
+      </c>
+      <c r="F6" t="n">
+        <v>19</v>
+      </c>
+      <c r="G6" t="n">
+        <v>99.26070038910505</v>
+      </c>
+      <c r="H6" t="n">
+        <v>99.14496696463273</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.01594710229482691</v>
+      </c>
+      <c r="J6" t="n">
+        <v>39.96841812133789</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>106</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2025</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2027</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2023</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
-        <v>2948</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2974</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2945</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="G7" t="n">
+        <v>99.85192497532083</v>
+      </c>
+      <c r="H7" t="n">
+        <v>99.9505928853755</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.001973359644795264</v>
+      </c>
+      <c r="J7" t="n">
+        <v>39.59288287162781</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>107</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2135</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2135</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2133</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>99.95313964386129</v>
+      </c>
+      <c r="H8" t="n">
+        <v>99.95313964386129</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.000936768149882904</v>
+      </c>
+      <c r="J8" t="n">
+        <v>40.49458837509155</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>108</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1766</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1762</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1754</v>
+      </c>
+      <c r="E9" t="n">
+        <v>11</v>
+      </c>
+      <c r="F9" t="n">
+        <v>7</v>
+      </c>
+      <c r="G9" t="n">
+        <v>99.60249858035208</v>
+      </c>
+      <c r="H9" t="n">
+        <v>99.37677053824362</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.01021566401816118</v>
+      </c>
+      <c r="J9" t="n">
+        <v>39.5079071521759</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>109</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2525</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2531</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2524</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>6</v>
+      </c>
+      <c r="G10" t="n">
+        <v>99.76284584980237</v>
+      </c>
+      <c r="H10" t="n">
+        <v>100</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.002370604504148558</v>
+      </c>
+      <c r="J10" t="n">
+        <v>39.46697068214417</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>111</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2122</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2124</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2120</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" t="n">
+        <v>99.85869053226565</v>
+      </c>
+      <c r="H11" t="n">
+        <v>99.95285242809996</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.001883239171374765</v>
+      </c>
+      <c r="J11" t="n">
+        <v>39.59419322013855</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>112</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2538</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2538</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2537</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>100</v>
+      </c>
+      <c r="H12" t="n">
+        <v>100</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>39.14341068267822</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>113</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1794</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1795</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1793</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>99.94425863991081</v>
+      </c>
+      <c r="H13" t="n">
+        <v>100</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.0005571030640668524</v>
+      </c>
+      <c r="J13" t="n">
+        <v>39.16032886505127</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>114</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1876</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1879</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1871</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4</v>
+      </c>
+      <c r="F14" t="n">
+        <v>7</v>
+      </c>
+      <c r="G14" t="n">
+        <v>99.6272630457934</v>
+      </c>
+      <c r="H14" t="n">
+        <v>99.78666666666666</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.005854177754124534</v>
+      </c>
+      <c r="J14" t="n">
+        <v>38.81715536117554</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>115</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1952</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1953</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1951</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>99.94877049180327</v>
+      </c>
+      <c r="H15" t="n">
+        <v>100</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.0005120327700972862</v>
+      </c>
+      <c r="J15" t="n">
+        <v>39.15442728996277</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>116</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2386</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2411</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2384</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="n">
+        <v>26</v>
+      </c>
+      <c r="G16" t="n">
+        <v>98.92116182572614</v>
+      </c>
+      <c r="H16" t="n">
+        <v>99.958071278826</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.01119867274989631</v>
+      </c>
+      <c r="J16" t="n">
+        <v>40.8009045124054</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>117</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1534</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1534</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1533</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>100</v>
+      </c>
+      <c r="H17" t="n">
+        <v>100</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>39.29325175285339</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>118</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2278</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2276</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2275</v>
+      </c>
+      <c r="E18" t="n">
         <v>2</v>
       </c>
-      <c r="F4" t="n">
-        <v>28</v>
-      </c>
-      <c r="G4" t="n">
-        <v>99.05819038008745</v>
-      </c>
-      <c r="H4" t="n">
-        <v>99.9321343739396</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.01008742434431742</v>
-      </c>
-      <c r="J4" t="n">
-        <v>64.55367970466614</v>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>100</v>
+      </c>
+      <c r="H18" t="n">
+        <v>99.91216512955643</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.0008787346221441124</v>
+      </c>
+      <c r="J18" t="n">
+        <v>40.34356570243835</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>119</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1989</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1987</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1986</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>100</v>
+      </c>
+      <c r="H19" t="n">
+        <v>99.89939637826961</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.001006542526421741</v>
+      </c>
+      <c r="J19" t="n">
+        <v>40.15085124969482</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>121</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1860</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1863</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1859</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" t="n">
+        <v>99.83888292158969</v>
+      </c>
+      <c r="H20" t="n">
+        <v>100</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.001610305958132045</v>
+      </c>
+      <c r="J20" t="n">
+        <v>38.92127299308777</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>122</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2475</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2475</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2474</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>100</v>
+      </c>
+      <c r="H21" t="n">
+        <v>100</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>39.36898040771484</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>123</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1518</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1517</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1516</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>100</v>
+      </c>
+      <c r="H22" t="n">
+        <v>99.9340804218853</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.0006591957811470006</v>
+      </c>
+      <c r="J22" t="n">
+        <v>39.15284609794617</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>124</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1619</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1619</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1617</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" t="n">
+        <v>99.93819530284301</v>
+      </c>
+      <c r="H23" t="n">
+        <v>99.93819530284301</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.001235330450895615</v>
+      </c>
+      <c r="J23" t="n">
+        <v>40.0520339012146</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>200</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2600</v>
+      </c>
+      <c r="C24" t="n">
+        <v>2601</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2597</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" t="n">
+        <v>3</v>
+      </c>
+      <c r="G24" t="n">
+        <v>99.88461538461539</v>
+      </c>
+      <c r="H24" t="n">
+        <v>99.92304732589457</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.001922337562475971</v>
+      </c>
+      <c r="J24" t="n">
+        <v>39.70689082145691</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>201</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1943</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1963</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1941</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" t="n">
+        <v>21</v>
+      </c>
+      <c r="G25" t="n">
+        <v>98.92966360856269</v>
+      </c>
+      <c r="H25" t="n">
+        <v>99.94850669412976</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.01120733571064697</v>
+      </c>
+      <c r="J25" t="n">
+        <v>39.56641626358032</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>202</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2130</v>
+      </c>
+      <c r="C26" t="n">
+        <v>2136</v>
+      </c>
+      <c r="D26" t="n">
+        <v>2126</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3</v>
+      </c>
+      <c r="F26" t="n">
+        <v>9</v>
+      </c>
+      <c r="G26" t="n">
+        <v>99.5784543325527</v>
+      </c>
+      <c r="H26" t="n">
+        <v>99.85908877407233</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.005617977528089887</v>
+      </c>
+      <c r="J26" t="n">
+        <v>38.67616510391235</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>203</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2666</v>
+      </c>
+      <c r="C27" t="n">
+        <v>2979</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2649</v>
+      </c>
+      <c r="E27" t="n">
+        <v>16</v>
+      </c>
+      <c r="F27" t="n">
+        <v>329</v>
+      </c>
+      <c r="G27" t="n">
+        <v>88.95231699126931</v>
+      </c>
+      <c r="H27" t="n">
+        <v>99.39962476547842</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.1158106747230614</v>
+      </c>
+      <c r="J27" t="n">
+        <v>40.62695813179016</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>205</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2634</v>
+      </c>
+      <c r="C28" t="n">
+        <v>2656</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2633</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>22</v>
+      </c>
+      <c r="G28" t="n">
+        <v>99.1713747645951</v>
+      </c>
+      <c r="H28" t="n">
+        <v>100</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.008283132530120483</v>
+      </c>
+      <c r="J28" t="n">
+        <v>40.22790122032166</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>207</v>
+      </c>
+      <c r="B29" t="n">
+        <v>2034</v>
+      </c>
+      <c r="C29" t="n">
+        <v>2331</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2008</v>
+      </c>
+      <c r="E29" t="n">
+        <v>25</v>
+      </c>
+      <c r="F29" t="n">
+        <v>322</v>
+      </c>
+      <c r="G29" t="n">
+        <v>86.18025751072962</v>
+      </c>
+      <c r="H29" t="n">
+        <v>98.77029021151009</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.1488631488631489</v>
+      </c>
+      <c r="J29" t="n">
+        <v>40.67711853981018</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>208</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2942</v>
+      </c>
+      <c r="C30" t="n">
+        <v>2953</v>
+      </c>
+      <c r="D30" t="n">
+        <v>2934</v>
+      </c>
+      <c r="E30" t="n">
+        <v>7</v>
+      </c>
+      <c r="F30" t="n">
+        <v>18</v>
+      </c>
+      <c r="G30" t="n">
+        <v>99.39024390243902</v>
+      </c>
+      <c r="H30" t="n">
+        <v>99.76198571914315</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.008465966813410091</v>
+      </c>
+      <c r="J30" t="n">
+        <v>40.27538371086121</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>209</v>
+      </c>
+      <c r="B31" t="n">
+        <v>2955</v>
+      </c>
+      <c r="C31" t="n">
+        <v>3005</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2954</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>50</v>
+      </c>
+      <c r="G31" t="n">
+        <v>98.33555259653795</v>
+      </c>
+      <c r="H31" t="n">
+        <v>100</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.01663893510815308</v>
+      </c>
+      <c r="J31" t="n">
+        <v>40.35048127174377</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>210</v>
+      </c>
+      <c r="B32" t="n">
+        <v>2603</v>
+      </c>
+      <c r="C32" t="n">
+        <v>2649</v>
+      </c>
+      <c r="D32" t="n">
+        <v>2601</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1</v>
+      </c>
+      <c r="F32" t="n">
+        <v>47</v>
+      </c>
+      <c r="G32" t="n">
+        <v>98.22507552870091</v>
+      </c>
+      <c r="H32" t="n">
+        <v>99.96156802459646</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.01812004530011325</v>
+      </c>
+      <c r="J32" t="n">
+        <v>39.36644601821899</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>212</v>
+      </c>
+      <c r="B33" t="n">
+        <v>2747</v>
+      </c>
+      <c r="C33" t="n">
+        <v>2747</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2746</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>100</v>
+      </c>
+      <c r="H33" t="n">
+        <v>100</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>41.27760362625122</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>213</v>
+      </c>
+      <c r="B34" t="n">
+        <v>3245</v>
+      </c>
+      <c r="C34" t="n">
+        <v>3248</v>
+      </c>
+      <c r="D34" t="n">
+        <v>3242</v>
+      </c>
+      <c r="E34" t="n">
+        <v>2</v>
+      </c>
+      <c r="F34" t="n">
+        <v>5</v>
+      </c>
+      <c r="G34" t="n">
+        <v>99.84601170311056</v>
+      </c>
+      <c r="H34" t="n">
+        <v>99.9383477188656</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.002155172413793103</v>
+      </c>
+      <c r="J34" t="n">
+        <v>42.40927863121033</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>214</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2251</v>
+      </c>
+      <c r="C35" t="n">
+        <v>2261</v>
+      </c>
+      <c r="D35" t="n">
+        <v>2250</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>10</v>
+      </c>
+      <c r="G35" t="n">
+        <v>99.5575221238938</v>
+      </c>
+      <c r="H35" t="n">
+        <v>100</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.004422821760283061</v>
+      </c>
+      <c r="J35" t="n">
+        <v>39.34359812736511</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>215</v>
+      </c>
+      <c r="B36" t="n">
+        <v>3330</v>
+      </c>
+      <c r="C36" t="n">
+        <v>3362</v>
+      </c>
+      <c r="D36" t="n">
+        <v>3329</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>32</v>
+      </c>
+      <c r="G36" t="n">
+        <v>99.04790240999702</v>
+      </c>
+      <c r="H36" t="n">
+        <v>100</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.009518143961927425</v>
+      </c>
+      <c r="J36" t="n">
+        <v>41.06773495674133</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>217</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2206</v>
+      </c>
+      <c r="C37" t="n">
+        <v>2208</v>
+      </c>
+      <c r="D37" t="n">
+        <v>2203</v>
+      </c>
+      <c r="E37" t="n">
+        <v>2</v>
+      </c>
+      <c r="F37" t="n">
+        <v>4</v>
+      </c>
+      <c r="G37" t="n">
+        <v>99.81875849569552</v>
+      </c>
+      <c r="H37" t="n">
+        <v>99.9092970521542</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.002717391304347826</v>
+      </c>
+      <c r="J37" t="n">
+        <v>40.26998114585876</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>219</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2155</v>
+      </c>
+      <c r="C38" t="n">
+        <v>2154</v>
+      </c>
+      <c r="D38" t="n">
+        <v>2153</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>100</v>
+      </c>
+      <c r="H38" t="n">
+        <v>99.9535747446611</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0.0004642525533890436</v>
+      </c>
+      <c r="J38" t="n">
+        <v>39.10490870475769</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>220</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2047</v>
+      </c>
+      <c r="C39" t="n">
+        <v>2047</v>
+      </c>
+      <c r="D39" t="n">
+        <v>2046</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>100</v>
+      </c>
+      <c r="H39" t="n">
+        <v>100</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>39.95473051071167</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>221</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2425</v>
+      </c>
+      <c r="C40" t="n">
+        <v>2427</v>
+      </c>
+      <c r="D40" t="n">
+        <v>2422</v>
+      </c>
+      <c r="E40" t="n">
+        <v>2</v>
+      </c>
+      <c r="F40" t="n">
+        <v>4</v>
+      </c>
+      <c r="G40" t="n">
+        <v>99.83511953833471</v>
+      </c>
+      <c r="H40" t="n">
+        <v>99.91749174917491</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0.002472187886279357</v>
+      </c>
+      <c r="J40" t="n">
+        <v>39.29483270645142</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>222</v>
+      </c>
+      <c r="B41" t="n">
+        <v>2462</v>
+      </c>
+      <c r="C41" t="n">
+        <v>2482</v>
+      </c>
+      <c r="D41" t="n">
+        <v>2457</v>
+      </c>
+      <c r="E41" t="n">
+        <v>4</v>
+      </c>
+      <c r="F41" t="n">
+        <v>24</v>
+      </c>
+      <c r="G41" t="n">
+        <v>99.03264812575574</v>
+      </c>
+      <c r="H41" t="n">
+        <v>99.83746444534742</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.0112812248186946</v>
+      </c>
+      <c r="J41" t="n">
+        <v>39.85415816307068</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>223</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2592</v>
+      </c>
+      <c r="C42" t="n">
+        <v>2605</v>
+      </c>
+      <c r="D42" t="n">
+        <v>2591</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>13</v>
+      </c>
+      <c r="G42" t="n">
+        <v>99.50076804915514</v>
+      </c>
+      <c r="H42" t="n">
+        <v>100</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0.004990403071017275</v>
+      </c>
+      <c r="J42" t="n">
+        <v>40.00896072387695</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>228</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2048</v>
+      </c>
+      <c r="C43" t="n">
+        <v>2052</v>
+      </c>
+      <c r="D43" t="n">
+        <v>2044</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3</v>
+      </c>
+      <c r="F43" t="n">
+        <v>7</v>
+      </c>
+      <c r="G43" t="n">
+        <v>99.65870307167235</v>
+      </c>
+      <c r="H43" t="n">
+        <v>99.85344406448461</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.004873294346978557</v>
+      </c>
+      <c r="J43" t="n">
+        <v>39.82225561141968</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>230</v>
+      </c>
+      <c r="B44" t="n">
+        <v>2255</v>
+      </c>
+      <c r="C44" t="n">
+        <v>2255</v>
+      </c>
+      <c r="D44" t="n">
+        <v>2254</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>100</v>
+      </c>
+      <c r="H44" t="n">
+        <v>100</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>39.86169648170471</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>231</v>
+      </c>
+      <c r="B45" t="n">
+        <v>1570</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1570</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1569</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>100</v>
+      </c>
+      <c r="H45" t="n">
+        <v>100</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>39.54058933258057</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>232</v>
+      </c>
+      <c r="B46" t="n">
+        <v>1783</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1780</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1779</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>100</v>
+      </c>
+      <c r="H46" t="n">
+        <v>99.83164983164983</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.001685393258426966</v>
+      </c>
+      <c r="J46" t="n">
+        <v>39.39215779304504</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>233</v>
+      </c>
+      <c r="B47" t="n">
+        <v>2965</v>
+      </c>
+      <c r="C47" t="n">
+        <v>3077</v>
+      </c>
+      <c r="D47" t="n">
+        <v>2963</v>
+      </c>
+      <c r="E47" t="n">
+        <v>1</v>
+      </c>
+      <c r="F47" t="n">
+        <v>113</v>
+      </c>
+      <c r="G47" t="n">
+        <v>96.32639791937581</v>
+      </c>
+      <c r="H47" t="n">
+        <v>99.96626180836707</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.03704907377315567</v>
+      </c>
+      <c r="J47" t="n">
+        <v>40.9127402305603</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>234</v>
+      </c>
+      <c r="B48" t="n">
+        <v>2752</v>
+      </c>
+      <c r="C48" t="n">
+        <v>2752</v>
+      </c>
+      <c r="D48" t="n">
+        <v>2751</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>100</v>
+      </c>
+      <c r="H48" t="n">
+        <v>100</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="n">
+        <v>40.30082130432129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>